<commit_message>
crfb full score is in stimulus round 2 tab
</commit_message>
<xml_diff>
--- a/inst/extdata/projections.xlsx
+++ b/inst/extdata/projections.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/fim/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E53387-4490-AC42-89F8-C889A106BCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB1E712-8DEA-9F43-BCF9-1010424DE873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13440" yWindow="1100" windowWidth="33600" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="economic" sheetId="1" r:id="rId1"/>
-    <sheet name="budget" sheetId="3" r:id="rId2"/>
-    <sheet name="quarterly fmap" sheetId="7" r:id="rId3"/>
-    <sheet name="annual fmap" sheetId="8" r:id="rId4"/>
-    <sheet name="CARES" sheetId="6" r:id="rId5"/>
-    <sheet name="crrca" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId7"/>
-    <sheet name="1. Quarterly" sheetId="2" r:id="rId8"/>
+    <sheet name="pre-pandemic economic" sheetId="9" r:id="rId1"/>
+    <sheet name="economic" sheetId="1" r:id="rId2"/>
+    <sheet name="budget" sheetId="3" r:id="rId3"/>
+    <sheet name="quarterly fmap" sheetId="7" r:id="rId4"/>
+    <sheet name="annual fmap" sheetId="8" r:id="rId5"/>
+    <sheet name="CARES" sheetId="6" r:id="rId6"/>
+    <sheet name="crrca" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId8"/>
+    <sheet name="1. Quarterly" sheetId="2" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'1. Quarterly'!$A$5:$AZ$135</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'1. Quarterly'!$A:$D</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'1. Quarterly'!$A$5:$AZ$135</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">'1. Quarterly'!$A:$D</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="215">
   <si>
     <t>date</t>
   </si>
@@ -712,6 +713,12 @@
   <si>
     <t>unemployment_rate</t>
   </si>
+  <si>
+    <t>federal_purchases_growth</t>
+  </si>
+  <si>
+    <t>state_purchases_growth</t>
+  </si>
 </sst>
 </file>
 
@@ -1342,6 +1349,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="47" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="27" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="46" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1352,7 +1360,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1"/>
-    <xf numFmtId="164" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1713,14 +1720,544 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86381FD6-3DA6-864B-ACAE-10D968FEABB3}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B2" s="14">
+        <v>5.3959999999999999</v>
+      </c>
+      <c r="C2" s="14">
+        <v>3.8639999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>44012</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2.79</v>
+      </c>
+      <c r="C3" s="14">
+        <v>3.2149999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44104</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2.7240000000000002</v>
+      </c>
+      <c r="C4" s="14">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44196</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2.6549999999999998</v>
+      </c>
+      <c r="C5" s="14">
+        <v>3.7440000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>44286</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2.7839999999999998</v>
+      </c>
+      <c r="C6" s="14">
+        <v>3.734</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>44377</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2.7959999999999998</v>
+      </c>
+      <c r="C7" s="14">
+        <v>3.7170000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>44469</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2.7669999999999999</v>
+      </c>
+      <c r="C8" s="14">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>44561</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2.4209999999999998</v>
+      </c>
+      <c r="C9" s="14">
+        <v>3.7509999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>44651</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2.536</v>
+      </c>
+      <c r="C10" s="14">
+        <v>3.8479999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>44742</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2.512</v>
+      </c>
+      <c r="C11" s="14">
+        <v>3.911</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>44834</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2.5459999999999998</v>
+      </c>
+      <c r="C12" s="14">
+        <v>3.9390000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B13" s="14">
+        <v>2.5859999999999999</v>
+      </c>
+      <c r="C13" s="14">
+        <v>3.9849999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B14" s="14">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3.9830000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B15" s="14">
+        <v>2.6059999999999999</v>
+      </c>
+      <c r="C15" s="14">
+        <v>3.9590000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>45199</v>
+      </c>
+      <c r="B16" s="14">
+        <v>2.5960000000000001</v>
+      </c>
+      <c r="C16" s="14">
+        <v>3.9830000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>45291</v>
+      </c>
+      <c r="B17" s="14">
+        <v>2.6259999999999999</v>
+      </c>
+      <c r="C17" s="14">
+        <v>3.976</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B18" s="14">
+        <v>2.6269999999999998</v>
+      </c>
+      <c r="C18" s="14">
+        <v>3.9649999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>45473</v>
+      </c>
+      <c r="B19" s="14">
+        <v>2.6259999999999999</v>
+      </c>
+      <c r="C19" s="14">
+        <v>3.9409999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>45565</v>
+      </c>
+      <c r="B20" s="14">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="C20" s="14">
+        <v>3.9470000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>45657</v>
+      </c>
+      <c r="B21" s="14">
+        <v>2.5659999999999998</v>
+      </c>
+      <c r="C21" s="14">
+        <v>3.9289999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>45747</v>
+      </c>
+      <c r="B22" s="14">
+        <v>2.4710000000000001</v>
+      </c>
+      <c r="C22" s="14">
+        <v>3.8860000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B23" s="14">
+        <v>2.46</v>
+      </c>
+      <c r="C23" s="14">
+        <v>3.847</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B24" s="14">
+        <v>2.4529999999999998</v>
+      </c>
+      <c r="C24" s="14">
+        <v>3.839</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>46022</v>
+      </c>
+      <c r="B25" s="14">
+        <v>2.552</v>
+      </c>
+      <c r="C25" s="14">
+        <v>3.819</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>46112</v>
+      </c>
+      <c r="B26" s="14">
+        <v>2.5019999999999998</v>
+      </c>
+      <c r="C26" s="14">
+        <v>3.8039999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>46203</v>
+      </c>
+      <c r="B27" s="14">
+        <v>2.5390000000000001</v>
+      </c>
+      <c r="C27" s="14">
+        <v>3.786</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>46295</v>
+      </c>
+      <c r="B28" s="14">
+        <v>2.5339999999999998</v>
+      </c>
+      <c r="C28" s="14">
+        <v>3.7989999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B29" s="14">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="C29" s="14">
+        <v>3.794</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>46477</v>
+      </c>
+      <c r="B30" s="14">
+        <v>2.4809999999999999</v>
+      </c>
+      <c r="C30" s="14">
+        <v>3.7879999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>46568</v>
+      </c>
+      <c r="B31" s="14">
+        <v>2.4729999999999999</v>
+      </c>
+      <c r="C31" s="14">
+        <v>3.7610000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>46660</v>
+      </c>
+      <c r="B32" s="14">
+        <v>2.5129999999999999</v>
+      </c>
+      <c r="C32" s="14">
+        <v>3.7509999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>46752</v>
+      </c>
+      <c r="B33" s="14">
+        <v>2.536</v>
+      </c>
+      <c r="C33" s="14">
+        <v>3.7349999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>46843</v>
+      </c>
+      <c r="B34" s="14">
+        <v>2.5289999999999999</v>
+      </c>
+      <c r="C34" s="14">
+        <v>3.7229999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>46934</v>
+      </c>
+      <c r="B35" s="14">
+        <v>2.5209999999999999</v>
+      </c>
+      <c r="C35" s="14">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>47026</v>
+      </c>
+      <c r="B36" s="14">
+        <v>2.508</v>
+      </c>
+      <c r="C36" s="14">
+        <v>3.7320000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>47118</v>
+      </c>
+      <c r="B37" s="14">
+        <v>2.496</v>
+      </c>
+      <c r="C37" s="14">
+        <v>3.7250000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>47208</v>
+      </c>
+      <c r="B38" s="14">
+        <v>2.4390000000000001</v>
+      </c>
+      <c r="C38" s="14">
+        <v>3.7149999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>47299</v>
+      </c>
+      <c r="B39" s="14">
+        <v>2.5179999999999998</v>
+      </c>
+      <c r="C39" s="14">
+        <v>3.7029999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>47391</v>
+      </c>
+      <c r="B40" s="14">
+        <v>2.4689999999999999</v>
+      </c>
+      <c r="C40" s="14">
+        <v>3.673</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>47483</v>
+      </c>
+      <c r="B41" s="14">
+        <v>2.4710000000000001</v>
+      </c>
+      <c r="C41" s="14">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>47573</v>
+      </c>
+      <c r="B42" s="14">
+        <v>2.5150000000000001</v>
+      </c>
+      <c r="C42" s="14">
+        <v>3.6349999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>47664</v>
+      </c>
+      <c r="B43" s="14">
+        <v>2.5179999999999998</v>
+      </c>
+      <c r="C43" s="14">
+        <v>3.6309999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>47756</v>
+      </c>
+      <c r="B44" s="14">
+        <v>2.5209999999999999</v>
+      </c>
+      <c r="C44" s="14">
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>47848</v>
+      </c>
+      <c r="B45" s="14">
+        <v>2.5680000000000001</v>
+      </c>
+      <c r="C45" s="14">
+        <v>3.6269999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>47938</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>48029</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>48121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>48213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1830,51 +2367,51 @@
       <c r="P2">
         <v>243.83</v>
       </c>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
-      <c r="AQ2" s="37"/>
-      <c r="AR2" s="37"/>
-      <c r="AS2" s="37"/>
-      <c r="AT2" s="37"/>
-      <c r="AU2" s="37"/>
-      <c r="AV2" s="37"/>
-      <c r="AW2" s="37"/>
-      <c r="AX2" s="37"/>
-      <c r="AY2" s="37"/>
-      <c r="AZ2" s="37"/>
-      <c r="BA2" s="37"/>
-      <c r="BB2" s="37"/>
-      <c r="BC2" s="37"/>
-      <c r="BD2" s="37"/>
-      <c r="BE2" s="37"/>
-      <c r="BF2" s="37"/>
-      <c r="BG2" s="37"/>
-      <c r="BH2" s="37"/>
-      <c r="BI2" s="37"/>
-      <c r="BJ2" s="37"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="33"/>
+      <c r="AV2" s="33"/>
+      <c r="AW2" s="33"/>
+      <c r="AX2" s="33"/>
+      <c r="AY2" s="33"/>
+      <c r="AZ2" s="33"/>
+      <c r="BA2" s="33"/>
+      <c r="BB2" s="33"/>
+      <c r="BC2" s="33"/>
+      <c r="BD2" s="33"/>
+      <c r="BE2" s="33"/>
+      <c r="BF2" s="33"/>
+      <c r="BG2" s="33"/>
+      <c r="BH2" s="33"/>
+      <c r="BI2" s="33"/>
+      <c r="BJ2" s="33"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -2625,7 +3162,7 @@
       <c r="P17" s="14">
         <v>260.59899999999999</v>
       </c>
-      <c r="Q17" s="37">
+      <c r="Q17" s="33">
         <v>6.8</v>
       </c>
     </row>
@@ -2678,7 +3215,7 @@
       <c r="P18" s="3">
         <v>261.77999999999997</v>
       </c>
-      <c r="Q18" s="37">
+      <c r="Q18" s="33">
         <v>6</v>
       </c>
     </row>
@@ -2731,7 +3268,7 @@
       <c r="P19" s="3">
         <v>263.077</v>
       </c>
-      <c r="Q19" s="37">
+      <c r="Q19" s="33">
         <v>6</v>
       </c>
     </row>
@@ -2784,7 +3321,7 @@
       <c r="P20" s="3">
         <v>264.58</v>
       </c>
-      <c r="Q20" s="37">
+      <c r="Q20" s="33">
         <v>5.6</v>
       </c>
     </row>
@@ -2837,7 +3374,7 @@
       <c r="P21" s="3">
         <v>265.661</v>
       </c>
-      <c r="Q21" s="37">
+      <c r="Q21" s="33">
         <v>5.3</v>
       </c>
     </row>
@@ -2890,7 +3427,7 @@
       <c r="P22" s="3">
         <v>267.07100000000003</v>
       </c>
-      <c r="Q22" s="37">
+      <c r="Q22" s="33">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -2943,7 +3480,7 @@
       <c r="P23" s="3">
         <v>268.524</v>
       </c>
-      <c r="Q23" s="37">
+      <c r="Q23" s="33">
         <v>5</v>
       </c>
     </row>
@@ -2996,7 +3533,7 @@
       <c r="P24" s="3">
         <v>269.99900000000002</v>
       </c>
-      <c r="Q24" s="37">
+      <c r="Q24" s="33">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -3049,7 +3586,7 @@
       <c r="P25" s="3">
         <v>271.512</v>
       </c>
-      <c r="Q25" s="37">
+      <c r="Q25" s="33">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -3102,7 +3639,7 @@
       <c r="P26" s="3">
         <v>273.03699999999998</v>
       </c>
-      <c r="Q26" s="37">
+      <c r="Q26" s="33">
         <v>4.8</v>
       </c>
     </row>
@@ -3155,7 +3692,7 @@
       <c r="P27" s="3">
         <v>274.58699999999999</v>
       </c>
-      <c r="Q27" s="37">
+      <c r="Q27" s="33">
         <v>4.8</v>
       </c>
     </row>
@@ -3208,7 +3745,7 @@
       <c r="P28" s="3">
         <v>276.15100000000001</v>
       </c>
-      <c r="Q28" s="37">
+      <c r="Q28" s="33">
         <v>4.7</v>
       </c>
     </row>
@@ -3261,7 +3798,7 @@
       <c r="P29" s="3">
         <v>277.72500000000002</v>
       </c>
-      <c r="Q29" s="37">
+      <c r="Q29" s="33">
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -3314,7 +3851,7 @@
       <c r="P30" s="3">
         <v>279.31700000000001</v>
       </c>
-      <c r="Q30" s="37">
+      <c r="Q30" s="33">
         <v>4.5</v>
       </c>
     </row>
@@ -3367,7 +3904,7 @@
       <c r="P31" s="3">
         <v>280.93099999999998</v>
       </c>
-      <c r="Q31" s="37">
+      <c r="Q31" s="33">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -3420,7 +3957,7 @@
       <c r="P32" s="3">
         <v>282.57100000000003</v>
       </c>
-      <c r="Q32" s="37">
+      <c r="Q32" s="33">
         <v>4.3</v>
       </c>
     </row>
@@ -3473,7 +4010,7 @@
       <c r="P33" s="3">
         <v>284.23099999999999</v>
       </c>
-      <c r="Q33" s="37">
+      <c r="Q33" s="33">
         <v>4.2</v>
       </c>
     </row>
@@ -3526,7 +4063,7 @@
       <c r="P34" s="3">
         <v>285.90300000000002</v>
       </c>
-      <c r="Q34" s="37">
+      <c r="Q34" s="33">
         <v>4.2</v>
       </c>
     </row>
@@ -3579,7 +4116,7 @@
       <c r="P35" s="3">
         <v>287.589</v>
       </c>
-      <c r="Q35" s="37">
+      <c r="Q35" s="33">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -3632,7 +4169,7 @@
       <c r="P36" s="3">
         <v>289.291</v>
       </c>
-      <c r="Q36" s="37">
+      <c r="Q36" s="33">
         <v>4</v>
       </c>
     </row>
@@ -3685,7 +4222,7 @@
       <c r="P37" s="3">
         <v>291.00799999999998</v>
       </c>
-      <c r="Q37" s="37">
+      <c r="Q37" s="33">
         <v>4</v>
       </c>
     </row>
@@ -3738,7 +4275,7 @@
       <c r="P38" s="3">
         <v>292.74700000000001</v>
       </c>
-      <c r="Q38" s="37">
+      <c r="Q38" s="33">
         <v>3.9</v>
       </c>
     </row>
@@ -3791,7 +4328,7 @@
       <c r="P39" s="3">
         <v>294.50099999999998</v>
       </c>
-      <c r="Q39" s="37">
+      <c r="Q39" s="33">
         <v>3.9</v>
       </c>
     </row>
@@ -3844,7 +4381,7 @@
       <c r="P40" s="3">
         <v>296.27</v>
       </c>
-      <c r="Q40" s="37">
+      <c r="Q40" s="33">
         <v>3.9</v>
       </c>
     </row>
@@ -3897,7 +4434,7 @@
       <c r="P41" s="3">
         <v>298.05500000000001</v>
       </c>
-      <c r="Q41" s="37">
+      <c r="Q41" s="33">
         <v>3.9</v>
       </c>
     </row>
@@ -3950,7 +4487,7 @@
       <c r="P42" s="3">
         <v>299.85899999999998</v>
       </c>
-      <c r="Q42" s="37">
+      <c r="Q42" s="33">
         <v>3.9</v>
       </c>
     </row>
@@ -4003,7 +4540,7 @@
       <c r="P43" s="3">
         <v>301.67599999999999</v>
       </c>
-      <c r="Q43" s="37">
+      <c r="Q43" s="33">
         <v>3.9</v>
       </c>
     </row>
@@ -4056,7 +4593,7 @@
       <c r="P44" s="3">
         <v>303.51</v>
       </c>
-      <c r="Q44" s="37">
+      <c r="Q44" s="33">
         <v>4</v>
       </c>
     </row>
@@ -4109,7 +4646,7 @@
       <c r="P45" s="3">
         <v>305.36</v>
       </c>
-      <c r="Q45" s="37">
+      <c r="Q45" s="33">
         <v>4</v>
       </c>
     </row>
@@ -4162,7 +4699,7 @@
       <c r="P46" s="3">
         <v>307.21699999999998</v>
       </c>
-      <c r="Q46" s="37">
+      <c r="Q46" s="33">
         <v>4</v>
       </c>
     </row>
@@ -4215,7 +4752,7 @@
       <c r="P47" s="3">
         <v>309.08699999999999</v>
       </c>
-      <c r="Q47" s="37">
+      <c r="Q47" s="33">
         <v>4</v>
       </c>
     </row>
@@ -4268,7 +4805,7 @@
       <c r="P48" s="3">
         <v>310.971</v>
       </c>
-      <c r="Q48" s="37">
+      <c r="Q48" s="33">
         <v>4</v>
       </c>
     </row>
@@ -4321,7 +4858,7 @@
       <c r="P49" s="3">
         <v>312.86900000000003</v>
       </c>
-      <c r="Q49" s="37">
+      <c r="Q49" s="33">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4374,7 +4911,7 @@
       <c r="P50" s="3">
         <v>314.762</v>
       </c>
-      <c r="Q50" s="37">
+      <c r="Q50" s="33">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4427,7 +4964,7 @@
       <c r="P51" s="3">
         <v>316.654</v>
       </c>
-      <c r="Q51" s="37">
+      <c r="Q51" s="33">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4480,7 +5017,7 @@
       <c r="P52" s="3">
         <v>318.54700000000003</v>
       </c>
-      <c r="Q52" s="37">
+      <c r="Q52" s="33">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4533,7 +5070,7 @@
       <c r="P53" s="3">
         <v>320.44</v>
       </c>
-      <c r="Q53" s="37">
+      <c r="Q53" s="33">
         <v>4.2</v>
       </c>
     </row>
@@ -4586,7 +5123,7 @@
       <c r="P54" s="3">
         <v>322.33199999999999</v>
       </c>
-      <c r="Q54" s="37">
+      <c r="Q54" s="33">
         <v>4.2</v>
       </c>
     </row>
@@ -4639,7 +5176,7 @@
       <c r="P55" s="3">
         <v>324.226</v>
       </c>
-      <c r="Q55" s="37">
+      <c r="Q55" s="33">
         <v>4.3</v>
       </c>
     </row>
@@ -4692,7 +5229,7 @@
       <c r="P56" s="3">
         <v>326.12200000000001</v>
       </c>
-      <c r="Q56" s="37">
+      <c r="Q56" s="33">
         <v>4.3</v>
       </c>
     </row>
@@ -4745,7 +5282,7 @@
       <c r="P57" s="3">
         <v>328.017</v>
       </c>
-      <c r="Q57" s="37">
+      <c r="Q57" s="33">
         <v>4.3</v>
       </c>
     </row>
@@ -4798,7 +5335,7 @@
       <c r="P58" s="3">
         <v>329.91500000000002</v>
       </c>
-      <c r="Q58" s="37">
+      <c r="Q58" s="33">
         <v>4.3</v>
       </c>
     </row>
@@ -4851,7 +5388,7 @@
       <c r="P59" s="3">
         <v>331.815</v>
       </c>
-      <c r="Q59" s="37">
+      <c r="Q59" s="33">
         <v>4.3</v>
       </c>
     </row>
@@ -4904,7 +5441,7 @@
       <c r="P60" s="3">
         <v>333.71899999999999</v>
       </c>
-      <c r="Q60" s="37">
+      <c r="Q60" s="33">
         <v>4.3</v>
       </c>
     </row>
@@ -4957,7 +5494,7 @@
       <c r="P61" s="3">
         <v>335.62799999999999</v>
       </c>
-      <c r="Q61" s="37">
+      <c r="Q61" s="33">
         <v>4.3</v>
       </c>
     </row>
@@ -4966,7 +5503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77260E8A-45C6-C74E-A071-E1E958901B15}">
   <dimension ref="A1:J16"/>
   <sheetViews>
@@ -5497,12 +6034,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DE4D24-926E-5240-89B6-F8FE59F1901D}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5728,7 +6265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B036E1FF-8773-7847-8D8D-5866CBDF4EC4}">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -5871,7 +6408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE6E772-7745-4345-AD59-C84EFCAA345D}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -6116,7 +6653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46AA86B-2BB2-174B-844E-5456E2801ADC}">
   <dimension ref="A1:O12"/>
   <sheetViews>
@@ -6643,7 +7180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E42683-B4AF-4746-955F-5BBF64474D4E}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -6745,7 +7282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7511D70-80B4-5E47-A7B7-55F3EFCB84BC}">
   <dimension ref="A1:BL135"/>
   <sheetViews>
@@ -6775,27 +7312,27 @@
       </c>
     </row>
     <row r="2" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="4" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -27633,12 +28170,12 @@
       </c>
     </row>
     <row r="130" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="36" t="s">
+      <c r="A130" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B130" s="36"/>
-      <c r="C130" s="36"/>
-      <c r="D130" s="36"/>
+      <c r="B130" s="37"/>
+      <c r="C130" s="37"/>
+      <c r="D130" s="37"/>
     </row>
     <row r="131" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C131" s="8"/>

</xml_diff>

<commit_message>
may update with cbo # pulled in from projections.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/projections.xlsx
+++ b/inst/extdata/projections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsalwati\Downloads\Hutchins Fiscal Impact Measure\fim\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA3D794-3DCF-44F6-AD6C-629E6134975E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0D213E1-11F1-4D06-9944-E15B378E3F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="251">
   <si>
     <t>date</t>
   </si>
@@ -771,6 +771,63 @@
   <si>
     <t xml:space="preserve">    "gsh", "Components of GDP (Real)", "Government Consumption Expenditures and Gross Investment", "State and local "</t>
   </si>
+  <si>
+    <t xml:space="preserve">Economic 10 yr Projection, Quarterly </t>
+  </si>
+  <si>
+    <t>"gftfp"</t>
+  </si>
+  <si>
+    <t>Social Security; Subtotal + Major Health Care Programs; Subtotal + Income Security Programs; Subtotal - Major Health Care Programs; Medicaid</t>
+  </si>
+  <si>
+    <t>"yptmd"</t>
+  </si>
+  <si>
+    <t>Major Health Care Programs; Medicaid</t>
+  </si>
+  <si>
+    <t>"yptmr"</t>
+  </si>
+  <si>
+    <t>Major Health Care Programs; Medicare</t>
+  </si>
+  <si>
+    <t>"yptu"</t>
+  </si>
+  <si>
+    <t>Income Security Programs; Unemployment Compensation</t>
+  </si>
+  <si>
+    <t>Budget 10 yr Projection, CBO's Baseline Budget Projections, by Category</t>
+  </si>
+  <si>
+    <t>Budget 10 yr Projection, Mandatory Outlays Projected in CBO's Baseline, Adjusted to Exclude Effects of Timing Shifts</t>
+  </si>
+  <si>
+    <t>"gfrpt"</t>
+  </si>
+  <si>
+    <t>"gfrs"</t>
+  </si>
+  <si>
+    <t>"gfrcp"</t>
+  </si>
+  <si>
+    <t>"gfrpri"</t>
+  </si>
+  <si>
+    <t>Revenues;Individual income taxes</t>
+  </si>
+  <si>
+    <t>Revenues;Payroll taxes</t>
+  </si>
+  <si>
+    <t>Revenues;Corporate income taxes</t>
+  </si>
+  <si>
+    <t>Revenues;Other</t>
+  </si>
 </sst>
 </file>
 
@@ -781,7 +838,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -976,8 +1033,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1181,6 +1247,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1369,7 +1441,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1"/>
@@ -1406,6 +1478,9 @@
     <xf numFmtId="0" fontId="26" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="27" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="19" fillId="36" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="19" fillId="36" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="46" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1416,9 +1491,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1"/>
-    <xf numFmtId="1" fontId="19" fillId="36" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="36" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1780,96 +1865,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9440D-BB32-4FF5-9B05-8B4462DE649B}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
         <v>231</v>
       </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+    </row>
+    <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B23" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B25" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>243</v>
+      </c>
+      <c r="B27" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>246</v>
+      </c>
+      <c r="B30" t="s">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A26:C26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1901,27 +2192,27 @@
       </c>
     </row>
     <row r="2" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="4" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -22759,12 +23050,12 @@
       </c>
     </row>
     <row r="130" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="35" t="s">
+      <c r="A130" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B130" s="35"/>
-      <c r="C130" s="35"/>
-      <c r="D130" s="35"/>
+      <c r="B130" s="38"/>
+      <c r="C130" s="38"/>
+      <c r="D130" s="38"/>
     </row>
     <row r="131" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C131" s="6"/>
@@ -22998,10 +23289,10 @@
       <c r="A10" s="1">
         <v>44651</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="33">
         <v>2.298</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="33">
         <v>9.2159999999999993</v>
       </c>
     </row>
@@ -23009,10 +23300,10 @@
       <c r="A11" s="1">
         <v>44742</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="33">
         <v>4.2320000000000002</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="33">
         <v>9.843</v>
       </c>
     </row>
@@ -23020,10 +23311,10 @@
       <c r="A12" s="1">
         <v>44834</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="33">
         <v>4.1929999999999996</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="33">
         <v>7.6760000000000002</v>
       </c>
     </row>
@@ -23031,10 +23322,10 @@
       <c r="A13" s="1">
         <v>44926</v>
       </c>
-      <c r="B13" s="37">
+      <c r="B13" s="33">
         <v>3.786</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="33">
         <v>5.7149999999999999</v>
       </c>
     </row>
@@ -23042,10 +23333,10 @@
       <c r="A14" s="1">
         <v>45016</v>
       </c>
-      <c r="B14" s="37">
+      <c r="B14" s="33">
         <v>4.0339999999999998</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="33">
         <v>4.9859999999999998</v>
       </c>
     </row>
@@ -23053,10 +23344,10 @@
       <c r="A15" s="1">
         <v>45107</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="33">
         <v>3.6819999999999999</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="33">
         <v>4.2220000000000004</v>
       </c>
     </row>
@@ -23064,10 +23355,10 @@
       <c r="A16" s="1">
         <v>45199</v>
       </c>
-      <c r="B16" s="37">
+      <c r="B16" s="33">
         <v>3.3159999999999998</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="33">
         <v>3.7879999999999998</v>
       </c>
     </row>
@@ -23075,10 +23366,10 @@
       <c r="A17" s="1">
         <v>45291</v>
       </c>
-      <c r="B17" s="37">
+      <c r="B17" s="33">
         <v>2.9569999999999999</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="33">
         <v>3.6309999999999998</v>
       </c>
     </row>
@@ -23086,10 +23377,10 @@
       <c r="A18" s="1">
         <v>45382</v>
       </c>
-      <c r="B18" s="37">
+      <c r="B18" s="33">
         <v>3.2949999999999999</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="33">
         <v>3.5049999999999999</v>
       </c>
     </row>
@@ -23097,10 +23388,10 @@
       <c r="A19" s="1">
         <v>45473</v>
       </c>
-      <c r="B19" s="37">
+      <c r="B19" s="33">
         <v>3.1269999999999998</v>
       </c>
-      <c r="C19" s="37">
+      <c r="C19" s="33">
         <v>3.4809999999999999</v>
       </c>
     </row>
@@ -23108,10 +23399,10 @@
       <c r="A20" s="1">
         <v>45565</v>
       </c>
-      <c r="B20" s="37">
+      <c r="B20" s="33">
         <v>3.125</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="33">
         <v>3.5430000000000001</v>
       </c>
     </row>
@@ -23119,10 +23410,10 @@
       <c r="A21" s="1">
         <v>45657</v>
       </c>
-      <c r="B21" s="37">
+      <c r="B21" s="33">
         <v>3.113</v>
       </c>
-      <c r="C21" s="37">
+      <c r="C21" s="33">
         <v>3.633</v>
       </c>
     </row>
@@ -23130,10 +23421,10 @@
       <c r="A22" s="1">
         <v>45747</v>
       </c>
-      <c r="B22" s="37">
+      <c r="B22" s="33">
         <v>2.5430000000000001</v>
       </c>
-      <c r="C22" s="37">
+      <c r="C22" s="33">
         <v>3.8759999999999999</v>
       </c>
     </row>
@@ -23141,10 +23432,10 @@
       <c r="A23" s="1">
         <v>45838</v>
       </c>
-      <c r="B23" s="37">
+      <c r="B23" s="33">
         <v>2.61</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="33">
         <v>3.98</v>
       </c>
     </row>
@@ -23152,10 +23443,10 @@
       <c r="A24" s="1">
         <v>45930</v>
       </c>
-      <c r="B24" s="37">
+      <c r="B24" s="33">
         <v>2.673</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="33">
         <v>4.0709999999999997</v>
       </c>
     </row>
@@ -23163,10 +23454,10 @@
       <c r="A25" s="1">
         <v>46022</v>
       </c>
-      <c r="B25" s="37">
+      <c r="B25" s="33">
         <v>2.7309999999999999</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="33">
         <v>4.0750000000000002</v>
       </c>
     </row>
@@ -23174,10 +23465,10 @@
       <c r="A26" s="1">
         <v>46112</v>
       </c>
-      <c r="B26" s="37">
+      <c r="B26" s="33">
         <v>2.5009999999999999</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="33">
         <v>4.032</v>
       </c>
     </row>
@@ -23185,10 +23476,10 @@
       <c r="A27" s="1">
         <v>46203</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B27" s="33">
         <v>2.59</v>
       </c>
-      <c r="C27" s="37">
+      <c r="C27" s="33">
         <v>3.9910000000000001</v>
       </c>
     </row>
@@ -23196,10 +23487,10 @@
       <c r="A28" s="1">
         <v>46295</v>
       </c>
-      <c r="B28" s="37">
+      <c r="B28" s="33">
         <v>2.661</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="33">
         <v>3.9529999999999998</v>
       </c>
     </row>
@@ -23207,10 +23498,10 @@
       <c r="A29" s="1">
         <v>46387</v>
       </c>
-      <c r="B29" s="37">
+      <c r="B29" s="33">
         <v>2.6659999999999999</v>
       </c>
-      <c r="C29" s="37">
+      <c r="C29" s="33">
         <v>3.923</v>
       </c>
     </row>
@@ -23218,10 +23509,10 @@
       <c r="A30" s="1">
         <v>46477</v>
       </c>
-      <c r="B30" s="37">
+      <c r="B30" s="33">
         <v>2.5910000000000002</v>
       </c>
-      <c r="C30" s="37">
+      <c r="C30" s="33">
         <v>3.8959999999999999</v>
       </c>
     </row>
@@ -23229,10 +23520,10 @@
       <c r="A31" s="1">
         <v>46568</v>
       </c>
-      <c r="B31" s="37">
+      <c r="B31" s="33">
         <v>2.5939999999999999</v>
       </c>
-      <c r="C31" s="37">
+      <c r="C31" s="33">
         <v>3.891</v>
       </c>
     </row>
@@ -23240,10 +23531,10 @@
       <c r="A32" s="1">
         <v>46660</v>
       </c>
-      <c r="B32" s="37">
+      <c r="B32" s="33">
         <v>2.5960000000000001</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C32" s="33">
         <v>3.8620000000000001</v>
       </c>
     </row>
@@ -23251,10 +23542,10 @@
       <c r="A33" s="1">
         <v>46752</v>
       </c>
-      <c r="B33" s="37">
+      <c r="B33" s="33">
         <v>2.6150000000000002</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="33">
         <v>3.8380000000000001</v>
       </c>
     </row>
@@ -23262,10 +23553,10 @@
       <c r="A34" s="1">
         <v>46843</v>
       </c>
-      <c r="B34" s="37">
+      <c r="B34" s="33">
         <v>2.5190000000000001</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="33">
         <v>3.8039999999999998</v>
       </c>
     </row>
@@ -23273,10 +23564,10 @@
       <c r="A35" s="1">
         <v>46934</v>
       </c>
-      <c r="B35" s="37">
+      <c r="B35" s="33">
         <v>2.5030000000000001</v>
       </c>
-      <c r="C35" s="37">
+      <c r="C35" s="33">
         <v>3.7970000000000002</v>
       </c>
     </row>
@@ -23284,10 +23575,10 @@
       <c r="A36" s="1">
         <v>47026</v>
       </c>
-      <c r="B36" s="37">
+      <c r="B36" s="33">
         <v>2.4790000000000001</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="33">
         <v>3.78</v>
       </c>
     </row>
@@ -23295,10 +23586,10 @@
       <c r="A37" s="1">
         <v>47118</v>
       </c>
-      <c r="B37" s="37">
+      <c r="B37" s="33">
         <v>2.4700000000000002</v>
       </c>
-      <c r="C37" s="37">
+      <c r="C37" s="33">
         <v>3.766</v>
       </c>
     </row>
@@ -23306,10 +23597,10 @@
       <c r="A38" s="1">
         <v>47208</v>
       </c>
-      <c r="B38" s="37">
+      <c r="B38" s="33">
         <v>2.4620000000000002</v>
       </c>
-      <c r="C38" s="37">
+      <c r="C38" s="33">
         <v>3.74</v>
       </c>
     </row>
@@ -23317,10 +23608,10 @@
       <c r="A39" s="1">
         <v>47299</v>
       </c>
-      <c r="B39" s="37">
+      <c r="B39" s="33">
         <v>2.4460000000000002</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="33">
         <v>3.746</v>
       </c>
     </row>
@@ -23328,10 +23619,10 @@
       <c r="A40" s="1">
         <v>47391</v>
       </c>
-      <c r="B40" s="37">
+      <c r="B40" s="33">
         <v>2.4380000000000002</v>
       </c>
-      <c r="C40" s="37">
+      <c r="C40" s="33">
         <v>3.7570000000000001</v>
       </c>
     </row>
@@ -23339,10 +23630,10 @@
       <c r="A41" s="1">
         <v>47483</v>
       </c>
-      <c r="B41" s="37">
+      <c r="B41" s="33">
         <v>2.4380000000000002</v>
       </c>
-      <c r="C41" s="37">
+      <c r="C41" s="33">
         <v>3.7709999999999999</v>
       </c>
     </row>
@@ -23350,10 +23641,10 @@
       <c r="A42" s="1">
         <v>47573</v>
       </c>
-      <c r="B42" s="37">
+      <c r="B42" s="33">
         <v>2.4350000000000001</v>
       </c>
-      <c r="C42" s="37">
+      <c r="C42" s="33">
         <v>3.7749999999999999</v>
       </c>
     </row>
@@ -23361,10 +23652,10 @@
       <c r="A43" s="1">
         <v>47664</v>
       </c>
-      <c r="B43" s="37">
+      <c r="B43" s="33">
         <v>2.431</v>
       </c>
-      <c r="C43" s="37">
+      <c r="C43" s="33">
         <v>3.7810000000000001</v>
       </c>
     </row>
@@ -23372,10 +23663,10 @@
       <c r="A44" s="1">
         <v>47756</v>
       </c>
-      <c r="B44" s="37">
+      <c r="B44" s="33">
         <v>2.4279999999999999</v>
       </c>
-      <c r="C44" s="37">
+      <c r="C44" s="33">
         <v>3.7879999999999998</v>
       </c>
     </row>
@@ -23383,10 +23674,10 @@
       <c r="A45" s="1">
         <v>47848</v>
       </c>
-      <c r="B45" s="37">
+      <c r="B45" s="33">
         <v>2.4239999999999999</v>
       </c>
-      <c r="C45" s="37">
+      <c r="C45" s="33">
         <v>3.7879999999999998</v>
       </c>
     </row>
@@ -23394,10 +23685,10 @@
       <c r="A46" s="1">
         <v>47938</v>
       </c>
-      <c r="B46" s="37">
+      <c r="B46" s="33">
         <v>2.3719999999999999</v>
       </c>
-      <c r="C46" s="37">
+      <c r="C46" s="33">
         <v>3.8069999999999999</v>
       </c>
     </row>
@@ -23405,10 +23696,10 @@
       <c r="A47" s="1">
         <v>48029</v>
       </c>
-      <c r="B47" s="37">
+      <c r="B47" s="33">
         <v>2.3679999999999999</v>
       </c>
-      <c r="C47" s="37">
+      <c r="C47" s="33">
         <v>3.7909999999999999</v>
       </c>
     </row>
@@ -23416,10 +23707,10 @@
       <c r="A48" s="1">
         <v>48121</v>
       </c>
-      <c r="B48" s="37">
+      <c r="B48" s="33">
         <v>2.3679999999999999</v>
       </c>
-      <c r="C48" s="37">
+      <c r="C48" s="33">
         <v>3.7909999999999999</v>
       </c>
     </row>
@@ -23427,42 +23718,42 @@
       <c r="A49" s="1">
         <v>48213</v>
       </c>
-      <c r="B49" s="37">
+      <c r="B49" s="33">
         <v>2.3690000000000002</v>
       </c>
-      <c r="C49" s="37">
+      <c r="C49" s="33">
         <v>3.7839999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="37">
+      <c r="B50" s="33">
         <v>2.3690000000000002</v>
       </c>
-      <c r="C50" s="37">
+      <c r="C50" s="33">
         <v>3.79</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="37">
+      <c r="B51" s="33">
         <v>2.37</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="33">
         <v>3.7909999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="37">
+      <c r="B52" s="33">
         <v>2.371</v>
       </c>
-      <c r="C52" s="37">
+      <c r="C52" s="33">
         <v>3.7869999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="37">
+      <c r="B53" s="33">
         <v>2.4249999999999998</v>
       </c>
-      <c r="C53" s="37">
+      <c r="C53" s="33">
         <v>3.79</v>
       </c>
     </row>
@@ -23479,7 +23770,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D62" sqref="D62"/>
+      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24649,52 +24940,52 @@
       <c r="A22" s="1">
         <v>44651</v>
       </c>
-      <c r="B22" s="36">
+      <c r="B22" s="32">
         <v>24422.799999999999</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="32">
         <v>19876.099999999999</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="32">
         <v>20005.5</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="32">
         <v>24577</v>
       </c>
-      <c r="F22" s="37">
+      <c r="F22" s="33">
         <v>119.761</v>
       </c>
-      <c r="G22" s="37">
+      <c r="G22" s="33">
         <v>122.875</v>
       </c>
-      <c r="H22" s="36">
+      <c r="H22" s="32">
         <v>16690.7</v>
       </c>
-      <c r="I22" s="36">
+      <c r="I22" s="32">
         <v>13936.6</v>
       </c>
-      <c r="J22" s="36">
+      <c r="J22" s="32">
         <v>3352.7</v>
       </c>
-      <c r="K22" s="36">
+      <c r="K22" s="32">
         <v>1318.9</v>
       </c>
-      <c r="L22" s="36">
+      <c r="L22" s="32">
         <v>2033</v>
       </c>
-      <c r="M22" s="36">
+      <c r="M22" s="32">
         <v>4200.2</v>
       </c>
-      <c r="N22" s="36">
+      <c r="N22" s="32">
         <v>1575</v>
       </c>
-      <c r="O22" s="36">
+      <c r="O22" s="32">
         <v>2625.2</v>
       </c>
-      <c r="P22" s="37">
+      <c r="P22" s="33">
         <v>282.976</v>
       </c>
-      <c r="Q22" s="37">
+      <c r="Q22" s="33">
         <v>3.91</v>
       </c>
     </row>
@@ -24702,52 +24993,52 @@
       <c r="A23" s="1">
         <v>44742</v>
       </c>
-      <c r="B23" s="36">
+      <c r="B23" s="32">
         <v>24956.9</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="32">
         <v>20083.5</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="32">
         <v>20101.2</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="32">
         <v>24971.1</v>
       </c>
-      <c r="F23" s="37">
+      <c r="F23" s="33">
         <v>121.06699999999999</v>
       </c>
-      <c r="G23" s="37">
+      <c r="G23" s="33">
         <v>124.265</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H23" s="32">
         <v>16993</v>
       </c>
-      <c r="I23" s="36">
+      <c r="I23" s="32">
         <v>14036</v>
       </c>
-      <c r="J23" s="36">
+      <c r="J23" s="32">
         <v>3370.8</v>
       </c>
-      <c r="K23" s="36">
+      <c r="K23" s="32">
         <v>1321.6</v>
       </c>
-      <c r="L23" s="36">
+      <c r="L23" s="32">
         <v>2048</v>
       </c>
-      <c r="M23" s="36">
+      <c r="M23" s="32">
         <v>4278.8999999999996</v>
       </c>
-      <c r="N23" s="36">
+      <c r="N23" s="32">
         <v>1591.4</v>
       </c>
-      <c r="O23" s="36">
+      <c r="O23" s="32">
         <v>2687.5</v>
       </c>
-      <c r="P23" s="37">
+      <c r="P23" s="33">
         <v>286.52100000000002</v>
       </c>
-      <c r="Q23" s="37">
+      <c r="Q23" s="33">
         <v>3.85</v>
       </c>
     </row>
@@ -24755,52 +25046,52 @@
       <c r="A24" s="1">
         <v>44834</v>
       </c>
-      <c r="B24" s="36">
+      <c r="B24" s="32">
         <v>25388.3</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="32">
         <v>20268.900000000001</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="32">
         <v>20197.900000000001</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="32">
         <v>25289.599999999999</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="33">
         <v>121.98699999999999</v>
       </c>
-      <c r="G24" s="37">
+      <c r="G24" s="33">
         <v>125.25700000000001</v>
       </c>
-      <c r="H24" s="36">
+      <c r="H24" s="32">
         <v>17251.3</v>
       </c>
-      <c r="I24" s="36">
+      <c r="I24" s="32">
         <v>14141.9</v>
       </c>
-      <c r="J24" s="36">
+      <c r="J24" s="32">
         <v>3390.3</v>
       </c>
-      <c r="K24" s="36">
+      <c r="K24" s="32">
         <v>1325.4</v>
       </c>
-      <c r="L24" s="36">
+      <c r="L24" s="32">
         <v>2063.4</v>
       </c>
-      <c r="M24" s="36">
+      <c r="M24" s="32">
         <v>4345.5</v>
       </c>
-      <c r="N24" s="36">
+      <c r="N24" s="32">
         <v>1607.9</v>
       </c>
-      <c r="O24" s="36">
+      <c r="O24" s="32">
         <v>2737.7</v>
       </c>
-      <c r="P24" s="37">
+      <c r="P24" s="33">
         <v>289.08600000000001</v>
       </c>
-      <c r="Q24" s="37">
+      <c r="Q24" s="33">
         <v>3.72</v>
       </c>
     </row>
@@ -24808,52 +25099,52 @@
       <c r="A25" s="1">
         <v>44926</v>
       </c>
-      <c r="B25" s="36">
+      <c r="B25" s="32">
         <v>25773.5</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C25" s="32">
         <v>20430.7</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="32">
         <v>20295.5</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="32">
         <v>25591.4</v>
       </c>
-      <c r="F25" s="37">
+      <c r="F25" s="33">
         <v>122.816</v>
       </c>
-      <c r="G25" s="37">
+      <c r="G25" s="33">
         <v>126.15</v>
       </c>
-      <c r="H25" s="36">
+      <c r="H25" s="32">
         <v>17488.099999999999</v>
       </c>
-      <c r="I25" s="36">
+      <c r="I25" s="32">
         <v>14239.3</v>
       </c>
-      <c r="J25" s="36">
+      <c r="J25" s="32">
         <v>3404.4</v>
       </c>
-      <c r="K25" s="36">
+      <c r="K25" s="32">
         <v>1330.1</v>
       </c>
-      <c r="L25" s="36">
+      <c r="L25" s="32">
         <v>2072.6999999999998</v>
       </c>
-      <c r="M25" s="36">
+      <c r="M25" s="32">
         <v>4398.8</v>
       </c>
-      <c r="N25" s="36">
+      <c r="N25" s="32">
         <v>1622.9</v>
       </c>
-      <c r="O25" s="36">
+      <c r="O25" s="32">
         <v>2776</v>
       </c>
-      <c r="P25" s="37">
+      <c r="P25" s="33">
         <v>291.41000000000003</v>
       </c>
-      <c r="Q25" s="37">
+      <c r="Q25" s="33">
         <v>3.65</v>
       </c>
     </row>
@@ -24861,52 +25152,52 @@
       <c r="A26" s="1">
         <v>45016</v>
       </c>
-      <c r="B26" s="36">
+      <c r="B26" s="32">
         <v>26095.1</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="32">
         <v>20557.7</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="32">
         <v>20393.599999999999</v>
       </c>
-      <c r="E26" s="36">
+      <c r="E26" s="32">
         <v>25874.1</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F26" s="33">
         <v>123.57299999999999</v>
       </c>
-      <c r="G26" s="37">
+      <c r="G26" s="33">
         <v>126.935</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H26" s="32">
         <v>17692.3</v>
       </c>
-      <c r="I26" s="36">
+      <c r="I26" s="32">
         <v>14317.2</v>
       </c>
-      <c r="J26" s="36">
+      <c r="J26" s="32">
         <v>3417</v>
       </c>
-      <c r="K26" s="36">
+      <c r="K26" s="32">
         <v>1336.1</v>
       </c>
-      <c r="L26" s="36">
+      <c r="L26" s="32">
         <v>2079.5</v>
       </c>
-      <c r="M26" s="36">
+      <c r="M26" s="32">
         <v>4448.8999999999996</v>
       </c>
-      <c r="N26" s="36">
+      <c r="N26" s="32">
         <v>1639</v>
       </c>
-      <c r="O26" s="36">
+      <c r="O26" s="32">
         <v>2809.9</v>
       </c>
-      <c r="P26" s="37">
+      <c r="P26" s="33">
         <v>293.56099999999998</v>
       </c>
-      <c r="Q26" s="37">
+      <c r="Q26" s="33">
         <v>3.58</v>
       </c>
     </row>
@@ -24914,52 +25205,52 @@
       <c r="A27" s="1">
         <v>45107</v>
       </c>
-      <c r="B27" s="36">
+      <c r="B27" s="32">
         <v>26403.7</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="32">
         <v>20684.3</v>
       </c>
-      <c r="D27" s="36">
+      <c r="D27" s="32">
         <v>20492.099999999999</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="32">
         <v>26144.6</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="33">
         <v>124.288</v>
       </c>
-      <c r="G27" s="37">
+      <c r="G27" s="33">
         <v>127.651</v>
       </c>
-      <c r="H27" s="36">
+      <c r="H27" s="32">
         <v>17892.599999999999</v>
       </c>
-      <c r="I27" s="36">
+      <c r="I27" s="32">
         <v>14396</v>
       </c>
-      <c r="J27" s="36">
+      <c r="J27" s="32">
         <v>3427.2</v>
       </c>
-      <c r="K27" s="36">
+      <c r="K27" s="32">
         <v>1341.1</v>
       </c>
-      <c r="L27" s="36">
+      <c r="L27" s="32">
         <v>2084.6999999999998</v>
       </c>
-      <c r="M27" s="36">
+      <c r="M27" s="32">
         <v>4493</v>
       </c>
-      <c r="N27" s="36">
+      <c r="N27" s="32">
         <v>1653.9</v>
       </c>
-      <c r="O27" s="36">
+      <c r="O27" s="32">
         <v>2839.2</v>
       </c>
-      <c r="P27" s="37">
+      <c r="P27" s="33">
         <v>295.51600000000002</v>
       </c>
-      <c r="Q27" s="37">
+      <c r="Q27" s="33">
         <v>3.52</v>
       </c>
     </row>
@@ -24967,52 +25258,52 @@
       <c r="A28" s="1">
         <v>45199</v>
       </c>
-      <c r="B28" s="36">
+      <c r="B28" s="32">
         <v>26686.3</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C28" s="32">
         <v>20792.8</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="32">
         <v>20591.2</v>
       </c>
-      <c r="E28" s="36">
+      <c r="E28" s="32">
         <v>26413</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="33">
         <v>124.98699999999999</v>
       </c>
-      <c r="G28" s="37">
+      <c r="G28" s="33">
         <v>128.34299999999999</v>
       </c>
-      <c r="H28" s="36">
+      <c r="H28" s="32">
         <v>18086.3</v>
       </c>
-      <c r="I28" s="36">
+      <c r="I28" s="32">
         <v>14470.5</v>
       </c>
-      <c r="J28" s="36">
+      <c r="J28" s="32">
         <v>3435.1</v>
       </c>
-      <c r="K28" s="36">
+      <c r="K28" s="32">
         <v>1344.8</v>
       </c>
-      <c r="L28" s="36">
+      <c r="L28" s="32">
         <v>2088.9</v>
       </c>
-      <c r="M28" s="36">
+      <c r="M28" s="32">
         <v>4533.1000000000004</v>
       </c>
-      <c r="N28" s="36">
+      <c r="N28" s="32">
         <v>1667.4</v>
       </c>
-      <c r="O28" s="36">
+      <c r="O28" s="32">
         <v>2865.7</v>
       </c>
-      <c r="P28" s="37">
+      <c r="P28" s="33">
         <v>297.36500000000001</v>
       </c>
-      <c r="Q28" s="37">
+      <c r="Q28" s="33">
         <v>3.5310000000000001</v>
       </c>
     </row>
@@ -25020,52 +25311,52 @@
       <c r="A29" s="1">
         <v>45291</v>
       </c>
-      <c r="B29" s="36">
+      <c r="B29" s="32">
         <v>26931.4</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C29" s="32">
         <v>20872.400000000001</v>
       </c>
-      <c r="D29" s="36">
+      <c r="D29" s="32">
         <v>20690.8</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="32">
         <v>26681.9</v>
       </c>
-      <c r="F29" s="37">
+      <c r="F29" s="33">
         <v>125.67400000000001</v>
       </c>
-      <c r="G29" s="37">
+      <c r="G29" s="33">
         <v>129.029</v>
       </c>
-      <c r="H29" s="36">
+      <c r="H29" s="32">
         <v>18268.2</v>
       </c>
-      <c r="I29" s="36">
+      <c r="I29" s="32">
         <v>14536.1</v>
       </c>
-      <c r="J29" s="36">
+      <c r="J29" s="32">
         <v>3441.4</v>
       </c>
-      <c r="K29" s="36">
+      <c r="K29" s="32">
         <v>1347.2</v>
       </c>
-      <c r="L29" s="36">
+      <c r="L29" s="32">
         <v>2092.8000000000002</v>
       </c>
-      <c r="M29" s="36">
+      <c r="M29" s="32">
         <v>4571</v>
       </c>
-      <c r="N29" s="36">
+      <c r="N29" s="32">
         <v>1679.6</v>
       </c>
-      <c r="O29" s="36">
+      <c r="O29" s="32">
         <v>2891.3</v>
       </c>
-      <c r="P29" s="37">
+      <c r="P29" s="33">
         <v>299.15499999999997</v>
       </c>
-      <c r="Q29" s="37">
+      <c r="Q29" s="33">
         <v>3.5510000000000002</v>
       </c>
     </row>
@@ -25073,52 +25364,52 @@
       <c r="A30" s="1">
         <v>45382</v>
       </c>
-      <c r="B30" s="36">
+      <c r="B30" s="32">
         <v>27173.9</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C30" s="32">
         <v>20947</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D30" s="32">
         <v>20790.8</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="32">
         <v>26955.4</v>
       </c>
-      <c r="F30" s="37">
+      <c r="F30" s="33">
         <v>126.343</v>
       </c>
-      <c r="G30" s="37">
+      <c r="G30" s="33">
         <v>129.727</v>
       </c>
-      <c r="H30" s="36">
+      <c r="H30" s="32">
         <v>18446.3</v>
       </c>
-      <c r="I30" s="36">
+      <c r="I30" s="32">
         <v>14600.2</v>
       </c>
-      <c r="J30" s="36">
+      <c r="J30" s="32">
         <v>3448.3</v>
       </c>
-      <c r="K30" s="36">
+      <c r="K30" s="32">
         <v>1350.7</v>
       </c>
-      <c r="L30" s="36">
+      <c r="L30" s="32">
         <v>2096.3000000000002</v>
       </c>
-      <c r="M30" s="36">
+      <c r="M30" s="32">
         <v>4609.6000000000004</v>
       </c>
-      <c r="N30" s="36">
+      <c r="N30" s="32">
         <v>1693.3</v>
       </c>
-      <c r="O30" s="36">
+      <c r="O30" s="32">
         <v>2916.4</v>
       </c>
-      <c r="P30" s="37">
+      <c r="P30" s="33">
         <v>300.90600000000001</v>
       </c>
-      <c r="Q30" s="37">
+      <c r="Q30" s="33">
         <v>3.6219999999999999</v>
       </c>
     </row>
@@ -25126,52 +25417,52 @@
       <c r="A31" s="1">
         <v>45473</v>
       </c>
-      <c r="B31" s="36">
+      <c r="B31" s="32">
         <v>27411.1</v>
       </c>
-      <c r="C31" s="36">
+      <c r="C31" s="32">
         <v>21021.4</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="32">
         <v>20890.5</v>
       </c>
-      <c r="E31" s="36">
+      <c r="E31" s="32">
         <v>27223.9</v>
       </c>
-      <c r="F31" s="37">
+      <c r="F31" s="33">
         <v>127.001</v>
       </c>
-      <c r="G31" s="37">
+      <c r="G31" s="33">
         <v>130.39599999999999</v>
       </c>
-      <c r="H31" s="36">
+      <c r="H31" s="32">
         <v>18612.400000000001</v>
       </c>
-      <c r="I31" s="36">
+      <c r="I31" s="32">
         <v>14655.3</v>
       </c>
-      <c r="J31" s="36">
+      <c r="J31" s="32">
         <v>3454.8</v>
       </c>
-      <c r="K31" s="36">
+      <c r="K31" s="32">
         <v>1353.6</v>
       </c>
-      <c r="L31" s="36">
+      <c r="L31" s="32">
         <v>2099.9</v>
       </c>
-      <c r="M31" s="36">
+      <c r="M31" s="32">
         <v>4647.8</v>
       </c>
-      <c r="N31" s="36">
+      <c r="N31" s="32">
         <v>1706.4</v>
       </c>
-      <c r="O31" s="36">
+      <c r="O31" s="32">
         <v>2941.4</v>
       </c>
-      <c r="P31" s="37">
+      <c r="P31" s="33">
         <v>302.64600000000002</v>
       </c>
-      <c r="Q31" s="37">
+      <c r="Q31" s="33">
         <v>3.6850000000000001</v>
       </c>
     </row>
@@ -25179,52 +25470,52 @@
       <c r="A32" s="1">
         <v>45565</v>
       </c>
-      <c r="B32" s="36">
+      <c r="B32" s="32">
         <v>27646.6</v>
       </c>
-      <c r="C32" s="36">
+      <c r="C32" s="32">
         <v>21094.799999999999</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D32" s="32">
         <v>20990</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="32">
         <v>27492.2</v>
       </c>
-      <c r="F32" s="37">
+      <c r="F32" s="33">
         <v>127.65</v>
       </c>
-      <c r="G32" s="37">
+      <c r="G32" s="33">
         <v>131.059</v>
       </c>
-      <c r="H32" s="36">
+      <c r="H32" s="32">
         <v>18774.5</v>
       </c>
-      <c r="I32" s="36">
+      <c r="I32" s="32">
         <v>14707.8</v>
       </c>
-      <c r="J32" s="36">
+      <c r="J32" s="32">
         <v>3461.5</v>
       </c>
-      <c r="K32" s="36">
+      <c r="K32" s="32">
         <v>1356.5</v>
       </c>
-      <c r="L32" s="36">
+      <c r="L32" s="32">
         <v>2103.8000000000002</v>
       </c>
-      <c r="M32" s="36">
+      <c r="M32" s="32">
         <v>4686.7</v>
       </c>
-      <c r="N32" s="36">
+      <c r="N32" s="32">
         <v>1719.6</v>
       </c>
-      <c r="O32" s="36">
+      <c r="O32" s="32">
         <v>2967.1</v>
       </c>
-      <c r="P32" s="37">
+      <c r="P32" s="33">
         <v>304.37299999999999</v>
       </c>
-      <c r="Q32" s="37">
+      <c r="Q32" s="33">
         <v>3.722</v>
       </c>
     </row>
@@ -25232,52 +25523,52 @@
       <c r="A33" s="1">
         <v>45657</v>
       </c>
-      <c r="B33" s="36">
+      <c r="B33" s="32">
         <v>27893.1</v>
       </c>
-      <c r="C33" s="36">
+      <c r="C33" s="32">
         <v>21176.400000000001</v>
       </c>
-      <c r="D33" s="36">
+      <c r="D33" s="32">
         <v>21089.3</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="32">
         <v>27760.799999999999</v>
       </c>
-      <c r="F33" s="37">
+      <c r="F33" s="33">
         <v>128.29400000000001</v>
       </c>
-      <c r="G33" s="37">
+      <c r="G33" s="33">
         <v>131.71700000000001</v>
       </c>
-      <c r="H33" s="36">
+      <c r="H33" s="32">
         <v>18946.900000000001</v>
       </c>
-      <c r="I33" s="36">
+      <c r="I33" s="32">
         <v>14768.3</v>
       </c>
-      <c r="J33" s="36">
+      <c r="J33" s="32">
         <v>3468.5</v>
       </c>
-      <c r="K33" s="36">
+      <c r="K33" s="32">
         <v>1359.2</v>
       </c>
-      <c r="L33" s="36">
+      <c r="L33" s="32">
         <v>2108</v>
       </c>
-      <c r="M33" s="36">
+      <c r="M33" s="32">
         <v>4726.5</v>
       </c>
-      <c r="N33" s="36">
+      <c r="N33" s="32">
         <v>1732.8</v>
       </c>
-      <c r="O33" s="36">
+      <c r="O33" s="32">
         <v>2993.7</v>
       </c>
-      <c r="P33" s="37">
+      <c r="P33" s="33">
         <v>306.09899999999999</v>
       </c>
-      <c r="Q33" s="37">
+      <c r="Q33" s="33">
         <v>3.76</v>
       </c>
     </row>
@@ -25285,52 +25576,52 @@
       <c r="A34" s="1">
         <v>45747</v>
       </c>
-      <c r="B34" s="36">
+      <c r="B34" s="32">
         <v>28142.6</v>
       </c>
-      <c r="C34" s="36">
+      <c r="C34" s="32">
         <v>21257.7</v>
       </c>
-      <c r="D34" s="36">
+      <c r="D34" s="32">
         <v>21188.3</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="32">
         <v>28032.799999999999</v>
       </c>
-      <c r="F34" s="37">
+      <c r="F34" s="33">
         <v>128.94200000000001</v>
       </c>
-      <c r="G34" s="37">
+      <c r="G34" s="33">
         <v>132.387</v>
       </c>
-      <c r="H34" s="36">
+      <c r="H34" s="32">
         <v>19117.900000000001</v>
       </c>
-      <c r="I34" s="36">
+      <c r="I34" s="32">
         <v>14826.6</v>
       </c>
-      <c r="J34" s="36">
+      <c r="J34" s="32">
         <v>3474.5</v>
       </c>
-      <c r="K34" s="36">
+      <c r="K34" s="32">
         <v>1360.1</v>
       </c>
-      <c r="L34" s="36">
+      <c r="L34" s="32">
         <v>2113</v>
       </c>
-      <c r="M34" s="36">
+      <c r="M34" s="32">
         <v>4766</v>
       </c>
-      <c r="N34" s="36">
+      <c r="N34" s="32">
         <v>1743.7</v>
       </c>
-      <c r="O34" s="36">
+      <c r="O34" s="32">
         <v>3022.3</v>
       </c>
-      <c r="P34" s="37">
+      <c r="P34" s="33">
         <v>307.85399999999998</v>
       </c>
-      <c r="Q34" s="37">
+      <c r="Q34" s="33">
         <v>3.7989999999999999</v>
       </c>
     </row>
@@ -25338,52 +25629,52 @@
       <c r="A35" s="1">
         <v>45838</v>
       </c>
-      <c r="B35" s="36">
+      <c r="B35" s="32">
         <v>28400.2</v>
       </c>
-      <c r="C35" s="36">
+      <c r="C35" s="32">
         <v>21343.8</v>
       </c>
-      <c r="D35" s="36">
+      <c r="D35" s="32">
         <v>21287.1</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="32">
         <v>28306.2</v>
       </c>
-      <c r="F35" s="37">
+      <c r="F35" s="33">
         <v>129.589</v>
       </c>
-      <c r="G35" s="37">
+      <c r="G35" s="33">
         <v>133.06</v>
       </c>
-      <c r="H35" s="36">
+      <c r="H35" s="32">
         <v>19292.7</v>
       </c>
-      <c r="I35" s="36">
+      <c r="I35" s="32">
         <v>14887.5</v>
       </c>
-      <c r="J35" s="36">
+      <c r="J35" s="32">
         <v>3481</v>
       </c>
-      <c r="K35" s="36">
+      <c r="K35" s="32">
         <v>1361.2</v>
       </c>
-      <c r="L35" s="36">
+      <c r="L35" s="32">
         <v>2118.1999999999998</v>
       </c>
-      <c r="M35" s="36">
+      <c r="M35" s="32">
         <v>4806.8999999999996</v>
       </c>
-      <c r="N35" s="36">
+      <c r="N35" s="32">
         <v>1755</v>
       </c>
-      <c r="O35" s="36">
+      <c r="O35" s="32">
         <v>3052</v>
       </c>
-      <c r="P35" s="37">
+      <c r="P35" s="33">
         <v>309.61799999999999</v>
       </c>
-      <c r="Q35" s="37">
+      <c r="Q35" s="33">
         <v>3.8380000000000001</v>
       </c>
     </row>
@@ -25391,52 +25682,52 @@
       <c r="A36" s="1">
         <v>45930</v>
       </c>
-      <c r="B36" s="36">
+      <c r="B36" s="32">
         <v>28648.6</v>
       </c>
-      <c r="C36" s="36">
+      <c r="C36" s="32">
         <v>21421</v>
       </c>
-      <c r="D36" s="36">
+      <c r="D36" s="32">
         <v>21385.9</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E36" s="32">
         <v>28582.6</v>
       </c>
-      <c r="F36" s="37">
+      <c r="F36" s="33">
         <v>130.23599999999999</v>
       </c>
-      <c r="G36" s="37">
+      <c r="G36" s="33">
         <v>133.74</v>
       </c>
-      <c r="H36" s="36">
+      <c r="H36" s="32">
         <v>19460.400000000001</v>
       </c>
-      <c r="I36" s="36">
+      <c r="I36" s="32">
         <v>14942.4</v>
       </c>
-      <c r="J36" s="36">
+      <c r="J36" s="32">
         <v>3487.9</v>
       </c>
-      <c r="K36" s="36">
+      <c r="K36" s="32">
         <v>1362.5</v>
       </c>
-      <c r="L36" s="36">
+      <c r="L36" s="32">
         <v>2123.6999999999998</v>
       </c>
-      <c r="M36" s="36">
+      <c r="M36" s="32">
         <v>4849.1000000000004</v>
       </c>
-      <c r="N36" s="36">
+      <c r="N36" s="32">
         <v>1766.6</v>
       </c>
-      <c r="O36" s="36">
+      <c r="O36" s="32">
         <v>3082.6</v>
       </c>
-      <c r="P36" s="37">
+      <c r="P36" s="33">
         <v>311.38799999999998</v>
       </c>
-      <c r="Q36" s="37">
+      <c r="Q36" s="33">
         <v>3.8769999999999998</v>
       </c>
     </row>
@@ -25444,52 +25735,52 @@
       <c r="A37" s="1">
         <v>46022</v>
       </c>
-      <c r="B37" s="36">
+      <c r="B37" s="32">
         <v>28909.599999999999</v>
       </c>
-      <c r="C37" s="36">
+      <c r="C37" s="32">
         <v>21506.400000000001</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D37" s="32">
         <v>21484.6</v>
       </c>
-      <c r="E37" s="36">
+      <c r="E37" s="32">
         <v>28860.799999999999</v>
       </c>
-      <c r="F37" s="37">
+      <c r="F37" s="33">
         <v>130.88200000000001</v>
       </c>
-      <c r="G37" s="37">
+      <c r="G37" s="33">
         <v>134.423</v>
       </c>
-      <c r="H37" s="36">
+      <c r="H37" s="32">
         <v>19646.400000000001</v>
       </c>
-      <c r="I37" s="36">
+      <c r="I37" s="32">
         <v>15010.7</v>
       </c>
-      <c r="J37" s="36">
+      <c r="J37" s="32">
         <v>3494.8</v>
       </c>
-      <c r="K37" s="36">
+      <c r="K37" s="32">
         <v>1363.9</v>
       </c>
-      <c r="L37" s="36">
+      <c r="L37" s="32">
         <v>2129</v>
       </c>
-      <c r="M37" s="36">
+      <c r="M37" s="32">
         <v>4892</v>
       </c>
-      <c r="N37" s="36">
+      <c r="N37" s="32">
         <v>1778.5</v>
       </c>
-      <c r="O37" s="36">
+      <c r="O37" s="32">
         <v>3113.5</v>
       </c>
-      <c r="P37" s="37">
+      <c r="P37" s="33">
         <v>313.16800000000001</v>
       </c>
-      <c r="Q37" s="37">
+      <c r="Q37" s="33">
         <v>3.915</v>
       </c>
     </row>
@@ -25497,52 +25788,52 @@
       <c r="A38" s="1">
         <v>46112</v>
       </c>
-      <c r="B38" s="36">
+      <c r="B38" s="32">
         <v>29128.2</v>
       </c>
-      <c r="C38" s="36">
+      <c r="C38" s="32">
         <v>21558.5</v>
       </c>
-      <c r="D38" s="36">
+      <c r="D38" s="32">
         <v>21583.3</v>
       </c>
-      <c r="E38" s="36">
+      <c r="E38" s="32">
         <v>29141.5</v>
       </c>
-      <c r="F38" s="37">
+      <c r="F38" s="33">
         <v>131.53100000000001</v>
       </c>
-      <c r="G38" s="37">
+      <c r="G38" s="33">
         <v>135.11199999999999</v>
       </c>
-      <c r="H38" s="36">
+      <c r="H38" s="32">
         <v>19785.3</v>
       </c>
-      <c r="I38" s="36">
+      <c r="I38" s="32">
         <v>15042.2</v>
       </c>
-      <c r="J38" s="36">
+      <c r="J38" s="32">
         <v>3500.7</v>
       </c>
-      <c r="K38" s="36">
+      <c r="K38" s="32">
         <v>1364.6</v>
       </c>
-      <c r="L38" s="36">
+      <c r="L38" s="32">
         <v>2134.1</v>
       </c>
-      <c r="M38" s="36">
+      <c r="M38" s="32">
         <v>4934</v>
       </c>
-      <c r="N38" s="36">
+      <c r="N38" s="32">
         <v>1789.5</v>
       </c>
-      <c r="O38" s="36">
+      <c r="O38" s="32">
         <v>3144.4</v>
       </c>
-      <c r="P38" s="37">
+      <c r="P38" s="33">
         <v>314.96199999999999</v>
       </c>
-      <c r="Q38" s="37">
+      <c r="Q38" s="33">
         <v>3.9590000000000001</v>
       </c>
     </row>
@@ -25550,52 +25841,52 @@
       <c r="A39" s="1">
         <v>46203</v>
       </c>
-      <c r="B39" s="36">
+      <c r="B39" s="32">
         <v>29382.5</v>
       </c>
-      <c r="C39" s="36">
+      <c r="C39" s="32">
         <v>21635.8</v>
       </c>
-      <c r="D39" s="36">
+      <c r="D39" s="32">
         <v>21681.5</v>
       </c>
-      <c r="E39" s="36">
+      <c r="E39" s="32">
         <v>29423.9</v>
       </c>
-      <c r="F39" s="37">
+      <c r="F39" s="33">
         <v>132.18299999999999</v>
       </c>
-      <c r="G39" s="37">
+      <c r="G39" s="33">
         <v>135.804</v>
       </c>
-      <c r="H39" s="36">
+      <c r="H39" s="32">
         <v>19957.400000000001</v>
       </c>
-      <c r="I39" s="36">
+      <c r="I39" s="32">
         <v>15098.3</v>
       </c>
-      <c r="J39" s="36">
+      <c r="J39" s="32">
         <v>3506.6</v>
       </c>
-      <c r="K39" s="36">
+      <c r="K39" s="32">
         <v>1365.6</v>
       </c>
-      <c r="L39" s="36">
+      <c r="L39" s="32">
         <v>2138.8000000000002</v>
       </c>
-      <c r="M39" s="36">
+      <c r="M39" s="32">
         <v>4976.3999999999996</v>
       </c>
-      <c r="N39" s="36">
+      <c r="N39" s="32">
         <v>1801</v>
       </c>
-      <c r="O39" s="36">
+      <c r="O39" s="32">
         <v>3175.3</v>
       </c>
-      <c r="P39" s="37">
+      <c r="P39" s="33">
         <v>316.77100000000002</v>
       </c>
-      <c r="Q39" s="37">
+      <c r="Q39" s="33">
         <v>4.0039999999999996</v>
       </c>
     </row>
@@ -25603,52 +25894,52 @@
       <c r="A40" s="1">
         <v>46295</v>
       </c>
-      <c r="B40" s="36">
+      <c r="B40" s="32">
         <v>29645.7</v>
       </c>
-      <c r="C40" s="36">
+      <c r="C40" s="32">
         <v>21718.1</v>
       </c>
-      <c r="D40" s="36">
+      <c r="D40" s="32">
         <v>21779.5</v>
       </c>
-      <c r="E40" s="36">
+      <c r="E40" s="32">
         <v>29708.3</v>
       </c>
-      <c r="F40" s="37">
+      <c r="F40" s="33">
         <v>132.83799999999999</v>
       </c>
-      <c r="G40" s="37">
+      <c r="G40" s="33">
         <v>136.50200000000001</v>
       </c>
-      <c r="H40" s="36">
+      <c r="H40" s="32">
         <v>20130.2</v>
       </c>
-      <c r="I40" s="36">
+      <c r="I40" s="32">
         <v>15153.9</v>
       </c>
-      <c r="J40" s="36">
+      <c r="J40" s="32">
         <v>3512.4</v>
       </c>
-      <c r="K40" s="36">
+      <c r="K40" s="32">
         <v>1366.8</v>
       </c>
-      <c r="L40" s="36">
+      <c r="L40" s="32">
         <v>2143.3000000000002</v>
       </c>
-      <c r="M40" s="36">
+      <c r="M40" s="32">
         <v>5019.2</v>
       </c>
-      <c r="N40" s="36">
+      <c r="N40" s="32">
         <v>1812.9</v>
       </c>
-      <c r="O40" s="36">
+      <c r="O40" s="32">
         <v>3206.3</v>
       </c>
-      <c r="P40" s="37">
+      <c r="P40" s="33">
         <v>318.596</v>
       </c>
-      <c r="Q40" s="37">
+      <c r="Q40" s="33">
         <v>4.0549999999999997</v>
       </c>
     </row>
@@ -25656,52 +25947,52 @@
       <c r="A41" s="1">
         <v>46387</v>
       </c>
-      <c r="B41" s="36">
+      <c r="B41" s="32">
         <v>29910.9</v>
       </c>
-      <c r="C41" s="36">
+      <c r="C41" s="32">
         <v>21800</v>
       </c>
-      <c r="D41" s="36">
+      <c r="D41" s="32">
         <v>21877.4</v>
       </c>
-      <c r="E41" s="36">
+      <c r="E41" s="32">
         <v>29995.200000000001</v>
       </c>
-      <c r="F41" s="37">
+      <c r="F41" s="33">
         <v>133.49600000000001</v>
       </c>
-      <c r="G41" s="37">
+      <c r="G41" s="33">
         <v>137.20500000000001</v>
       </c>
-      <c r="H41" s="36">
+      <c r="H41" s="32">
         <v>20306.2</v>
       </c>
-      <c r="I41" s="36">
+      <c r="I41" s="32">
         <v>15211</v>
       </c>
-      <c r="J41" s="36">
+      <c r="J41" s="32">
         <v>3518</v>
       </c>
-      <c r="K41" s="36">
+      <c r="K41" s="32">
         <v>1368</v>
       </c>
-      <c r="L41" s="36">
+      <c r="L41" s="32">
         <v>2147.6</v>
       </c>
-      <c r="M41" s="36">
+      <c r="M41" s="32">
         <v>5062.1000000000004</v>
       </c>
-      <c r="N41" s="36">
+      <c r="N41" s="32">
         <v>1824.8</v>
       </c>
-      <c r="O41" s="36">
+      <c r="O41" s="32">
         <v>3237.3</v>
       </c>
-      <c r="P41" s="37">
+      <c r="P41" s="33">
         <v>320.43700000000001</v>
       </c>
-      <c r="Q41" s="37">
+      <c r="Q41" s="33">
         <v>4.101</v>
       </c>
     </row>
@@ -25709,52 +26000,52 @@
       <c r="A42" s="1">
         <v>46477</v>
       </c>
-      <c r="B42" s="36">
+      <c r="B42" s="32">
         <v>30191</v>
       </c>
-      <c r="C42" s="36">
+      <c r="C42" s="32">
         <v>21891.200000000001</v>
       </c>
-      <c r="D42" s="36">
+      <c r="D42" s="32">
         <v>21975.200000000001</v>
       </c>
-      <c r="E42" s="36">
+      <c r="E42" s="32">
         <v>30284.5</v>
       </c>
-      <c r="F42" s="37">
+      <c r="F42" s="33">
         <v>134.16</v>
       </c>
-      <c r="G42" s="37">
+      <c r="G42" s="33">
         <v>137.91399999999999</v>
       </c>
-      <c r="H42" s="36">
+      <c r="H42" s="32">
         <v>20502.900000000001</v>
       </c>
-      <c r="I42" s="36">
+      <c r="I42" s="32">
         <v>15282.4</v>
       </c>
-      <c r="J42" s="36">
+      <c r="J42" s="32">
         <v>3523.2</v>
       </c>
-      <c r="K42" s="36">
+      <c r="K42" s="32">
         <v>1368.9</v>
       </c>
-      <c r="L42" s="36">
+      <c r="L42" s="32">
         <v>2151.8000000000002</v>
       </c>
-      <c r="M42" s="36">
+      <c r="M42" s="32">
         <v>5104.8999999999996</v>
       </c>
-      <c r="N42" s="36">
+      <c r="N42" s="32">
         <v>1836.6</v>
       </c>
-      <c r="O42" s="36">
+      <c r="O42" s="32">
         <v>3268.4</v>
       </c>
-      <c r="P42" s="37">
+      <c r="P42" s="33">
         <v>322.29599999999999</v>
       </c>
-      <c r="Q42" s="37">
+      <c r="Q42" s="33">
         <v>4.149</v>
       </c>
     </row>
@@ -25762,52 +26053,52 @@
       <c r="A43" s="1">
         <v>46568</v>
       </c>
-      <c r="B43" s="36">
+      <c r="B43" s="32">
         <v>30471.3</v>
       </c>
-      <c r="C43" s="36">
+      <c r="C43" s="32">
         <v>21980.6</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D43" s="32">
         <v>22072.9</v>
       </c>
-      <c r="E43" s="36">
+      <c r="E43" s="32">
         <v>30576.1</v>
       </c>
-      <c r="F43" s="37">
+      <c r="F43" s="33">
         <v>134.828</v>
       </c>
-      <c r="G43" s="37">
+      <c r="G43" s="33">
         <v>138.62700000000001</v>
       </c>
-      <c r="H43" s="36">
+      <c r="H43" s="32">
         <v>20698.3</v>
       </c>
-      <c r="I43" s="36">
+      <c r="I43" s="32">
         <v>15351.6</v>
       </c>
-      <c r="J43" s="36">
+      <c r="J43" s="32">
         <v>3528.4</v>
       </c>
-      <c r="K43" s="36">
+      <c r="K43" s="32">
         <v>1369.9</v>
       </c>
-      <c r="L43" s="36">
+      <c r="L43" s="32">
         <v>2155.8000000000002</v>
       </c>
-      <c r="M43" s="36">
+      <c r="M43" s="32">
         <v>5148.1000000000004</v>
       </c>
-      <c r="N43" s="36">
+      <c r="N43" s="32">
         <v>1848.4</v>
       </c>
-      <c r="O43" s="36">
+      <c r="O43" s="32">
         <v>3299.7</v>
       </c>
-      <c r="P43" s="37">
+      <c r="P43" s="33">
         <v>324.17099999999999</v>
       </c>
-      <c r="Q43" s="37">
+      <c r="Q43" s="33">
         <v>4.1920000000000002</v>
       </c>
     </row>
@@ -25815,52 +26106,52 @@
       <c r="A44" s="1">
         <v>46660</v>
       </c>
-      <c r="B44" s="36">
+      <c r="B44" s="32">
         <v>30754</v>
       </c>
-      <c r="C44" s="36">
+      <c r="C44" s="32">
         <v>22070.2</v>
       </c>
-      <c r="D44" s="36">
+      <c r="D44" s="32">
         <v>22170.400000000001</v>
       </c>
-      <c r="E44" s="36">
+      <c r="E44" s="32">
         <v>30870</v>
       </c>
-      <c r="F44" s="37">
+      <c r="F44" s="33">
         <v>135.5</v>
       </c>
-      <c r="G44" s="37">
+      <c r="G44" s="33">
         <v>139.346</v>
       </c>
-      <c r="H44" s="36">
+      <c r="H44" s="32">
         <v>20899.5</v>
       </c>
-      <c r="I44" s="36">
+      <c r="I44" s="32">
         <v>15424</v>
       </c>
-      <c r="J44" s="36">
+      <c r="J44" s="32">
         <v>3533.3</v>
       </c>
-      <c r="K44" s="36">
+      <c r="K44" s="32">
         <v>1370.8</v>
       </c>
-      <c r="L44" s="36">
+      <c r="L44" s="32">
         <v>2159.6999999999998</v>
       </c>
-      <c r="M44" s="36">
+      <c r="M44" s="32">
         <v>5191.3999999999996</v>
       </c>
-      <c r="N44" s="36">
+      <c r="N44" s="32">
         <v>1860.2</v>
       </c>
-      <c r="O44" s="36">
+      <c r="O44" s="32">
         <v>3331.1</v>
       </c>
-      <c r="P44" s="37">
+      <c r="P44" s="33">
         <v>326.06099999999998</v>
       </c>
-      <c r="Q44" s="37">
+      <c r="Q44" s="33">
         <v>4.2469999999999999</v>
       </c>
     </row>
@@ -25868,52 +26159,52 @@
       <c r="A45" s="1">
         <v>46752</v>
       </c>
-      <c r="B45" s="36">
+      <c r="B45" s="32">
         <v>31038.799999999999</v>
       </c>
-      <c r="C45" s="36">
+      <c r="C45" s="32">
         <v>22159.7</v>
       </c>
-      <c r="D45" s="36">
+      <c r="D45" s="32">
         <v>22268.1</v>
       </c>
-      <c r="E45" s="36">
+      <c r="E45" s="32">
         <v>31166.3</v>
       </c>
-      <c r="F45" s="37">
+      <c r="F45" s="33">
         <v>136.17500000000001</v>
       </c>
-      <c r="G45" s="37">
+      <c r="G45" s="33">
         <v>140.06800000000001</v>
       </c>
-      <c r="H45" s="36">
+      <c r="H45" s="32">
         <v>21100.2</v>
       </c>
-      <c r="I45" s="36">
+      <c r="I45" s="32">
         <v>15494.9</v>
       </c>
-      <c r="J45" s="36">
+      <c r="J45" s="32">
         <v>3538.1</v>
       </c>
-      <c r="K45" s="36">
+      <c r="K45" s="32">
         <v>1371.9</v>
       </c>
-      <c r="L45" s="36">
+      <c r="L45" s="32">
         <v>2163.4</v>
       </c>
-      <c r="M45" s="36">
+      <c r="M45" s="32">
         <v>5234.8999999999996</v>
       </c>
-      <c r="N45" s="36">
+      <c r="N45" s="32">
         <v>1872.3</v>
       </c>
-      <c r="O45" s="36">
+      <c r="O45" s="32">
         <v>3362.6</v>
       </c>
-      <c r="P45" s="37">
+      <c r="P45" s="33">
         <v>327.96199999999999</v>
       </c>
-      <c r="Q45" s="37">
+      <c r="Q45" s="33">
         <v>4.3079999999999998</v>
       </c>
     </row>
@@ -25921,52 +26212,52 @@
       <c r="A46" s="1">
         <v>46843</v>
       </c>
-      <c r="B46" s="36">
+      <c r="B46" s="32">
         <v>31335.7</v>
       </c>
-      <c r="C46" s="36">
+      <c r="C46" s="32">
         <v>22256.400000000001</v>
       </c>
-      <c r="D46" s="36">
+      <c r="D46" s="32">
         <v>22366</v>
       </c>
-      <c r="E46" s="36">
+      <c r="E46" s="32">
         <v>31465.1</v>
       </c>
-      <c r="F46" s="37">
+      <c r="F46" s="33">
         <v>136.85499999999999</v>
       </c>
-      <c r="G46" s="37">
+      <c r="G46" s="33">
         <v>140.79400000000001</v>
       </c>
-      <c r="H46" s="36">
+      <c r="H46" s="32">
         <v>21316.5</v>
       </c>
-      <c r="I46" s="36">
+      <c r="I46" s="32">
         <v>15575.9</v>
       </c>
-      <c r="J46" s="36">
+      <c r="J46" s="32">
         <v>3542.5</v>
       </c>
-      <c r="K46" s="36">
+      <c r="K46" s="32">
         <v>1372.6</v>
       </c>
-      <c r="L46" s="36">
+      <c r="L46" s="32">
         <v>2166.9</v>
       </c>
-      <c r="M46" s="36">
+      <c r="M46" s="32">
         <v>5278.1</v>
       </c>
-      <c r="N46" s="36">
+      <c r="N46" s="32">
         <v>1884</v>
       </c>
-      <c r="O46" s="36">
+      <c r="O46" s="32">
         <v>3394.2</v>
       </c>
-      <c r="P46" s="37">
+      <c r="P46" s="33">
         <v>329.87799999999999</v>
       </c>
-      <c r="Q46" s="37">
+      <c r="Q46" s="33">
         <v>4.3780000000000001</v>
       </c>
     </row>
@@ -25974,52 +26265,52 @@
       <c r="A47" s="1">
         <v>46934</v>
       </c>
-      <c r="B47" s="36">
+      <c r="B47" s="32">
         <v>31633.8</v>
       </c>
-      <c r="C47" s="36">
+      <c r="C47" s="32">
         <v>22352.1</v>
       </c>
-      <c r="D47" s="36">
+      <c r="D47" s="32">
         <v>22464.400000000001</v>
       </c>
-      <c r="E47" s="36">
+      <c r="E47" s="32">
         <v>31767.200000000001</v>
       </c>
-      <c r="F47" s="37">
+      <c r="F47" s="33">
         <v>137.541</v>
       </c>
-      <c r="G47" s="37">
+      <c r="G47" s="33">
         <v>141.52500000000001</v>
       </c>
-      <c r="H47" s="36">
+      <c r="H47" s="32">
         <v>21534.9</v>
       </c>
-      <c r="I47" s="36">
+      <c r="I47" s="32">
         <v>15657</v>
       </c>
-      <c r="J47" s="36">
+      <c r="J47" s="32">
         <v>3546.8</v>
       </c>
-      <c r="K47" s="36">
+      <c r="K47" s="32">
         <v>1373.3</v>
       </c>
-      <c r="L47" s="36">
+      <c r="L47" s="32">
         <v>2170.4</v>
       </c>
-      <c r="M47" s="36">
+      <c r="M47" s="32">
         <v>5321.6</v>
       </c>
-      <c r="N47" s="36">
+      <c r="N47" s="32">
         <v>1895.7</v>
       </c>
-      <c r="O47" s="36">
+      <c r="O47" s="32">
         <v>3425.9</v>
       </c>
-      <c r="P47" s="37">
+      <c r="P47" s="33">
         <v>331.81099999999998</v>
       </c>
-      <c r="Q47" s="37">
+      <c r="Q47" s="33">
         <v>4.45</v>
       </c>
     </row>
@@ -26027,52 +26318,52 @@
       <c r="A48" s="1">
         <v>47026</v>
       </c>
-      <c r="B48" s="36">
+      <c r="B48" s="32">
         <v>31938.2</v>
       </c>
-      <c r="C48" s="36">
+      <c r="C48" s="32">
         <v>22450.5</v>
       </c>
-      <c r="D48" s="36">
+      <c r="D48" s="32">
         <v>22563.3</v>
       </c>
-      <c r="E48" s="36">
+      <c r="E48" s="32">
         <v>32072.5</v>
       </c>
-      <c r="F48" s="37">
+      <c r="F48" s="33">
         <v>138.232</v>
       </c>
-      <c r="G48" s="37">
+      <c r="G48" s="33">
         <v>142.261</v>
       </c>
-      <c r="H48" s="36">
+      <c r="H48" s="32">
         <v>21753.9</v>
       </c>
-      <c r="I48" s="36">
+      <c r="I48" s="32">
         <v>15737.3</v>
       </c>
-      <c r="J48" s="36">
+      <c r="J48" s="32">
         <v>3550.9</v>
       </c>
-      <c r="K48" s="36">
+      <c r="K48" s="32">
         <v>1373.9</v>
       </c>
-      <c r="L48" s="36">
+      <c r="L48" s="32">
         <v>2173.8000000000002</v>
       </c>
-      <c r="M48" s="36">
+      <c r="M48" s="32">
         <v>5365.2</v>
       </c>
-      <c r="N48" s="36">
+      <c r="N48" s="32">
         <v>1907.3</v>
       </c>
-      <c r="O48" s="36">
+      <c r="O48" s="32">
         <v>3457.9</v>
       </c>
-      <c r="P48" s="37">
+      <c r="P48" s="33">
         <v>333.76</v>
       </c>
-      <c r="Q48" s="37">
+      <c r="Q48" s="33">
         <v>4.5019999999999998</v>
       </c>
     </row>
@@ -26080,52 +26371,52 @@
       <c r="A49" s="1">
         <v>47118</v>
       </c>
-      <c r="B49" s="36">
+      <c r="B49" s="32">
         <v>32245.9</v>
       </c>
-      <c r="C49" s="36">
+      <c r="C49" s="32">
         <v>22549.4</v>
       </c>
-      <c r="D49" s="36">
+      <c r="D49" s="32">
         <v>22662.7</v>
       </c>
-      <c r="E49" s="36">
+      <c r="E49" s="32">
         <v>32381.1</v>
       </c>
-      <c r="F49" s="37">
+      <c r="F49" s="33">
         <v>138.92699999999999</v>
       </c>
-      <c r="G49" s="37">
+      <c r="G49" s="33">
         <v>143.001</v>
       </c>
-      <c r="H49" s="36">
+      <c r="H49" s="32">
         <v>21974.7</v>
       </c>
-      <c r="I49" s="36">
+      <c r="I49" s="32">
         <v>15817.4</v>
       </c>
-      <c r="J49" s="36">
+      <c r="J49" s="32">
         <v>3554.9</v>
       </c>
-      <c r="K49" s="36">
+      <c r="K49" s="32">
         <v>1374.5</v>
       </c>
-      <c r="L49" s="36">
+      <c r="L49" s="32">
         <v>2177</v>
       </c>
-      <c r="M49" s="36">
+      <c r="M49" s="32">
         <v>5409</v>
       </c>
-      <c r="N49" s="36">
+      <c r="N49" s="32">
         <v>1919</v>
       </c>
-      <c r="O49" s="36">
+      <c r="O49" s="32">
         <v>3490</v>
       </c>
-      <c r="P49" s="37">
+      <c r="P49" s="33">
         <v>335.72300000000001</v>
       </c>
-      <c r="Q49" s="37">
+      <c r="Q49" s="33">
         <v>4.53</v>
       </c>
     </row>
@@ -26133,52 +26424,52 @@
       <c r="A50" s="1">
         <v>47208</v>
       </c>
-      <c r="B50" s="36">
+      <c r="B50" s="32">
         <v>32557.200000000001</v>
       </c>
-      <c r="C50" s="36">
+      <c r="C50" s="32">
         <v>22649</v>
       </c>
-      <c r="D50" s="36">
+      <c r="D50" s="32">
         <v>22762.799999999999</v>
       </c>
-      <c r="E50" s="36">
+      <c r="E50" s="32">
         <v>32693.200000000001</v>
       </c>
-      <c r="F50" s="37">
+      <c r="F50" s="33">
         <v>139.62700000000001</v>
       </c>
-      <c r="G50" s="37">
+      <c r="G50" s="33">
         <v>143.74600000000001</v>
       </c>
-      <c r="H50" s="36">
+      <c r="H50" s="32">
         <v>22194.2</v>
       </c>
-      <c r="I50" s="36">
+      <c r="I50" s="32">
         <v>15895.3</v>
       </c>
-      <c r="J50" s="36">
+      <c r="J50" s="32">
         <v>3558.7</v>
       </c>
-      <c r="K50" s="36">
+      <c r="K50" s="32">
         <v>1375.1</v>
       </c>
-      <c r="L50" s="36">
+      <c r="L50" s="32">
         <v>2180.1</v>
       </c>
-      <c r="M50" s="36">
+      <c r="M50" s="32">
         <v>5452.8</v>
       </c>
-      <c r="N50" s="36">
+      <c r="N50" s="32">
         <v>1930.7</v>
       </c>
-      <c r="O50" s="36">
+      <c r="O50" s="32">
         <v>3522.2</v>
       </c>
-      <c r="P50" s="37">
+      <c r="P50" s="33">
         <v>337.69900000000001</v>
       </c>
-      <c r="Q50" s="37">
+      <c r="Q50" s="33">
         <v>4.5359999999999996</v>
       </c>
     </row>
@@ -26186,52 +26477,52 @@
       <c r="A51" s="1">
         <v>47299</v>
       </c>
-      <c r="B51" s="36">
+      <c r="B51" s="32">
         <v>32872</v>
       </c>
-      <c r="C51" s="36">
+      <c r="C51" s="32">
         <v>22749.200000000001</v>
       </c>
-      <c r="D51" s="36">
+      <c r="D51" s="32">
         <v>22863.5</v>
       </c>
-      <c r="E51" s="36">
+      <c r="E51" s="32">
         <v>33008.9</v>
       </c>
-      <c r="F51" s="37">
+      <c r="F51" s="33">
         <v>140.33000000000001</v>
       </c>
-      <c r="G51" s="37">
+      <c r="G51" s="33">
         <v>144.49700000000001</v>
       </c>
-      <c r="H51" s="36">
+      <c r="H51" s="32">
         <v>22419.7</v>
       </c>
-      <c r="I51" s="36">
+      <c r="I51" s="32">
         <v>15976.3</v>
       </c>
-      <c r="J51" s="36">
+      <c r="J51" s="32">
         <v>3562.4</v>
       </c>
-      <c r="K51" s="36">
+      <c r="K51" s="32">
         <v>1375.6</v>
       </c>
-      <c r="L51" s="36">
+      <c r="L51" s="32">
         <v>2183.1999999999998</v>
       </c>
-      <c r="M51" s="36">
+      <c r="M51" s="32">
         <v>5497.1</v>
       </c>
-      <c r="N51" s="36">
+      <c r="N51" s="32">
         <v>1942.4</v>
       </c>
-      <c r="O51" s="36">
+      <c r="O51" s="32">
         <v>3554.7</v>
       </c>
-      <c r="P51" s="37">
+      <c r="P51" s="33">
         <v>339.685</v>
       </c>
-      <c r="Q51" s="37">
+      <c r="Q51" s="33">
         <v>4.5389999999999997</v>
       </c>
     </row>
@@ -26239,52 +26530,52 @@
       <c r="A52" s="1">
         <v>47391</v>
       </c>
-      <c r="B52" s="36">
+      <c r="B52" s="32">
         <v>33189.5</v>
       </c>
-      <c r="C52" s="36">
+      <c r="C52" s="32">
         <v>22849.5</v>
       </c>
-      <c r="D52" s="36">
+      <c r="D52" s="32">
         <v>22964.3</v>
       </c>
-      <c r="E52" s="36">
+      <c r="E52" s="32">
         <v>33327.300000000003</v>
       </c>
-      <c r="F52" s="37">
+      <c r="F52" s="33">
         <v>141.03800000000001</v>
       </c>
-      <c r="G52" s="37">
+      <c r="G52" s="33">
         <v>145.25200000000001</v>
       </c>
-      <c r="H52" s="36">
+      <c r="H52" s="32">
         <v>22644.6</v>
       </c>
-      <c r="I52" s="36">
+      <c r="I52" s="32">
         <v>16055.6</v>
       </c>
-      <c r="J52" s="36">
+      <c r="J52" s="32">
         <v>3566.1</v>
       </c>
-      <c r="K52" s="36">
+      <c r="K52" s="32">
         <v>1376.1</v>
       </c>
-      <c r="L52" s="36">
+      <c r="L52" s="32">
         <v>2186.1999999999998</v>
       </c>
-      <c r="M52" s="36">
+      <c r="M52" s="32">
         <v>5541.7</v>
       </c>
-      <c r="N52" s="36">
+      <c r="N52" s="32">
         <v>1954.1</v>
       </c>
-      <c r="O52" s="36">
+      <c r="O52" s="32">
         <v>3587.6</v>
       </c>
-      <c r="P52" s="37">
+      <c r="P52" s="33">
         <v>341.68200000000002</v>
       </c>
-      <c r="Q52" s="37">
+      <c r="Q52" s="33">
         <v>4.5419999999999998</v>
       </c>
     </row>
@@ -26292,52 +26583,52 @@
       <c r="A53" s="1">
         <v>47483</v>
       </c>
-      <c r="B53" s="36">
+      <c r="B53" s="32">
         <v>33509.699999999997</v>
       </c>
-      <c r="C53" s="36">
+      <c r="C53" s="32">
         <v>22949.8</v>
       </c>
-      <c r="D53" s="36">
+      <c r="D53" s="32">
         <v>23065.1</v>
       </c>
-      <c r="E53" s="36">
+      <c r="E53" s="32">
         <v>33648.400000000001</v>
       </c>
-      <c r="F53" s="37">
+      <c r="F53" s="33">
         <v>141.749</v>
       </c>
-      <c r="G53" s="37">
+      <c r="G53" s="33">
         <v>146.01300000000001</v>
       </c>
-      <c r="H53" s="36">
+      <c r="H53" s="32">
         <v>22872.2</v>
       </c>
-      <c r="I53" s="36">
+      <c r="I53" s="32">
         <v>16135.6</v>
       </c>
-      <c r="J53" s="36">
+      <c r="J53" s="32">
         <v>3569.8</v>
       </c>
-      <c r="K53" s="36">
+      <c r="K53" s="32">
         <v>1376.6</v>
       </c>
-      <c r="L53" s="36">
+      <c r="L53" s="32">
         <v>2189.4</v>
       </c>
-      <c r="M53" s="36">
+      <c r="M53" s="32">
         <v>5586.9</v>
       </c>
-      <c r="N53" s="36">
+      <c r="N53" s="32">
         <v>1965.9</v>
       </c>
-      <c r="O53" s="36">
+      <c r="O53" s="32">
         <v>3621</v>
       </c>
-      <c r="P53" s="37">
+      <c r="P53" s="33">
         <v>343.68900000000002</v>
       </c>
-      <c r="Q53" s="37">
+      <c r="Q53" s="33">
         <v>4.5460000000000003</v>
       </c>
     </row>
@@ -26345,52 +26636,52 @@
       <c r="A54" s="1">
         <v>47573</v>
       </c>
-      <c r="B54" s="36">
+      <c r="B54" s="32">
         <v>33832.400000000001</v>
       </c>
-      <c r="C54" s="36">
+      <c r="C54" s="32">
         <v>23050.2</v>
       </c>
-      <c r="D54" s="36">
+      <c r="D54" s="32">
         <v>23166</v>
       </c>
-      <c r="E54" s="36">
+      <c r="E54" s="32">
         <v>33972</v>
       </c>
-      <c r="F54" s="37">
+      <c r="F54" s="33">
         <v>142.464</v>
       </c>
-      <c r="G54" s="37">
+      <c r="G54" s="33">
         <v>146.77699999999999</v>
       </c>
-      <c r="H54" s="36">
+      <c r="H54" s="32">
         <v>23102.400000000001</v>
       </c>
-      <c r="I54" s="36">
+      <c r="I54" s="32">
         <v>16216.3</v>
       </c>
-      <c r="J54" s="36">
+      <c r="J54" s="32">
         <v>3573.6</v>
       </c>
-      <c r="K54" s="36">
+      <c r="K54" s="32">
         <v>1377.1</v>
       </c>
-      <c r="L54" s="36">
+      <c r="L54" s="32">
         <v>2192.5</v>
       </c>
-      <c r="M54" s="36">
+      <c r="M54" s="32">
         <v>5632.5</v>
       </c>
-      <c r="N54" s="36">
+      <c r="N54" s="32">
         <v>1977.8</v>
       </c>
-      <c r="O54" s="36">
+      <c r="O54" s="32">
         <v>3654.7</v>
       </c>
-      <c r="P54" s="37">
+      <c r="P54" s="33">
         <v>345.702</v>
       </c>
-      <c r="Q54" s="37">
+      <c r="Q54" s="33">
         <v>4.5490000000000004</v>
       </c>
     </row>
@@ -26398,52 +26689,52 @@
       <c r="A55" s="1">
         <v>47664</v>
       </c>
-      <c r="B55" s="36">
+      <c r="B55" s="32">
         <v>34157.599999999999</v>
       </c>
-      <c r="C55" s="36">
+      <c r="C55" s="32">
         <v>23150.799999999999</v>
       </c>
-      <c r="D55" s="36">
+      <c r="D55" s="32">
         <v>23267.1</v>
       </c>
-      <c r="E55" s="36">
+      <c r="E55" s="32">
         <v>34298.1</v>
       </c>
-      <c r="F55" s="37">
+      <c r="F55" s="33">
         <v>143.18100000000001</v>
       </c>
-      <c r="G55" s="37">
+      <c r="G55" s="33">
         <v>147.54300000000001</v>
       </c>
-      <c r="H55" s="36">
+      <c r="H55" s="32">
         <v>23337.1</v>
       </c>
-      <c r="I55" s="36">
+      <c r="I55" s="32">
         <v>16299</v>
       </c>
-      <c r="J55" s="36">
+      <c r="J55" s="32">
         <v>3577.5</v>
       </c>
-      <c r="K55" s="36">
+      <c r="K55" s="32">
         <v>1377.6</v>
       </c>
-      <c r="L55" s="36">
+      <c r="L55" s="32">
         <v>2195.6999999999998</v>
       </c>
-      <c r="M55" s="36">
+      <c r="M55" s="32">
         <v>5678.5</v>
       </c>
-      <c r="N55" s="36">
+      <c r="N55" s="32">
         <v>1989.7</v>
       </c>
-      <c r="O55" s="36">
+      <c r="O55" s="32">
         <v>3688.8</v>
       </c>
-      <c r="P55" s="37">
+      <c r="P55" s="33">
         <v>347.72300000000001</v>
       </c>
-      <c r="Q55" s="37">
+      <c r="Q55" s="33">
         <v>4.5519999999999996</v>
       </c>
     </row>
@@ -26451,52 +26742,52 @@
       <c r="A56" s="1">
         <v>47756</v>
       </c>
-      <c r="B56" s="36">
+      <c r="B56" s="32">
         <v>34485.4</v>
       </c>
-      <c r="C56" s="36">
+      <c r="C56" s="32">
         <v>23251.5</v>
       </c>
-      <c r="D56" s="36">
+      <c r="D56" s="32">
         <v>23368.3</v>
       </c>
-      <c r="E56" s="36">
+      <c r="E56" s="32">
         <v>34626.699999999997</v>
       </c>
-      <c r="F56" s="37">
+      <c r="F56" s="33">
         <v>143.90100000000001</v>
       </c>
-      <c r="G56" s="37">
+      <c r="G56" s="33">
         <v>148.31399999999999</v>
       </c>
-      <c r="H56" s="36">
+      <c r="H56" s="32">
         <v>23573.200000000001</v>
       </c>
-      <c r="I56" s="36">
+      <c r="I56" s="32">
         <v>16381.5</v>
       </c>
-      <c r="J56" s="36">
+      <c r="J56" s="32">
         <v>3581.4</v>
       </c>
-      <c r="K56" s="36">
+      <c r="K56" s="32">
         <v>1378.1</v>
       </c>
-      <c r="L56" s="36">
+      <c r="L56" s="32">
         <v>2199</v>
       </c>
-      <c r="M56" s="36">
+      <c r="M56" s="32">
         <v>5724.9</v>
       </c>
-      <c r="N56" s="36">
+      <c r="N56" s="32">
         <v>2001.7</v>
       </c>
-      <c r="O56" s="36">
+      <c r="O56" s="32">
         <v>3723.2</v>
       </c>
-      <c r="P56" s="37">
+      <c r="P56" s="33">
         <v>349.75299999999999</v>
       </c>
-      <c r="Q56" s="37">
+      <c r="Q56" s="33">
         <v>4.5540000000000003</v>
       </c>
     </row>
@@ -26504,52 +26795,52 @@
       <c r="A57" s="1">
         <v>47848</v>
       </c>
-      <c r="B57" s="36">
+      <c r="B57" s="32">
         <v>34815.699999999997</v>
       </c>
-      <c r="C57" s="36">
+      <c r="C57" s="32">
         <v>23352.400000000001</v>
       </c>
-      <c r="D57" s="36">
+      <c r="D57" s="32">
         <v>23469.7</v>
       </c>
-      <c r="E57" s="36">
+      <c r="E57" s="32">
         <v>34957.9</v>
       </c>
-      <c r="F57" s="37">
+      <c r="F57" s="33">
         <v>144.62299999999999</v>
       </c>
-      <c r="G57" s="37">
+      <c r="G57" s="33">
         <v>149.08799999999999</v>
       </c>
-      <c r="H57" s="36">
+      <c r="H57" s="32">
         <v>23810.1</v>
       </c>
-      <c r="I57" s="36">
+      <c r="I57" s="32">
         <v>16463.5</v>
       </c>
-      <c r="J57" s="36">
+      <c r="J57" s="32">
         <v>3585.2</v>
       </c>
-      <c r="K57" s="36">
+      <c r="K57" s="32">
         <v>1378.5</v>
       </c>
-      <c r="L57" s="36">
+      <c r="L57" s="32">
         <v>2202.1999999999998</v>
       </c>
-      <c r="M57" s="36">
+      <c r="M57" s="32">
         <v>5771.7</v>
       </c>
-      <c r="N57" s="36">
+      <c r="N57" s="32">
         <v>2013.7</v>
       </c>
-      <c r="O57" s="36">
+      <c r="O57" s="32">
         <v>3758</v>
       </c>
-      <c r="P57" s="37">
+      <c r="P57" s="33">
         <v>351.78899999999999</v>
       </c>
-      <c r="Q57" s="37">
+      <c r="Q57" s="33">
         <v>4.5579999999999998</v>
       </c>
     </row>
@@ -26557,52 +26848,52 @@
       <c r="A58" s="1">
         <v>47938</v>
       </c>
-      <c r="B58" s="36">
+      <c r="B58" s="32">
         <v>35148.6</v>
       </c>
-      <c r="C58" s="36">
+      <c r="C58" s="32">
         <v>23453.5</v>
       </c>
-      <c r="D58" s="36">
+      <c r="D58" s="32">
         <v>23571.200000000001</v>
       </c>
-      <c r="E58" s="36">
+      <c r="E58" s="32">
         <v>35291.800000000003</v>
       </c>
-      <c r="F58" s="37">
+      <c r="F58" s="33">
         <v>145.34899999999999</v>
       </c>
-      <c r="G58" s="37">
+      <c r="G58" s="33">
         <v>149.86500000000001</v>
       </c>
-      <c r="H58" s="36">
+      <c r="H58" s="32">
         <v>24050.400000000001</v>
       </c>
-      <c r="I58" s="36">
+      <c r="I58" s="32">
         <v>16546.599999999999</v>
       </c>
-      <c r="J58" s="36">
+      <c r="J58" s="32">
         <v>3589</v>
       </c>
-      <c r="K58" s="36">
+      <c r="K58" s="32">
         <v>1378.8</v>
       </c>
-      <c r="L58" s="36">
+      <c r="L58" s="32">
         <v>2205.5</v>
       </c>
-      <c r="M58" s="36">
+      <c r="M58" s="32">
         <v>5818.8</v>
       </c>
-      <c r="N58" s="36">
+      <c r="N58" s="32">
         <v>2025.5</v>
       </c>
-      <c r="O58" s="36">
+      <c r="O58" s="32">
         <v>3793.3</v>
       </c>
-      <c r="P58" s="37">
+      <c r="P58" s="33">
         <v>353.83199999999999</v>
       </c>
-      <c r="Q58" s="37">
+      <c r="Q58" s="33">
         <v>4.5510000000000002</v>
       </c>
     </row>
@@ -26610,52 +26901,52 @@
       <c r="A59" s="1">
         <v>48029</v>
       </c>
-      <c r="B59" s="36">
+      <c r="B59" s="32">
         <v>35484.1</v>
       </c>
-      <c r="C59" s="36">
+      <c r="C59" s="32">
         <v>23554.7</v>
       </c>
-      <c r="D59" s="36">
+      <c r="D59" s="32">
         <v>23672.9</v>
       </c>
-      <c r="E59" s="36">
+      <c r="E59" s="32">
         <v>35628.199999999997</v>
       </c>
-      <c r="F59" s="37">
+      <c r="F59" s="33">
         <v>146.077</v>
       </c>
-      <c r="G59" s="37">
+      <c r="G59" s="33">
         <v>150.64500000000001</v>
       </c>
-      <c r="H59" s="36">
+      <c r="H59" s="32">
         <v>24294.799999999999</v>
       </c>
-      <c r="I59" s="36">
+      <c r="I59" s="32">
         <v>16631.400000000001</v>
       </c>
-      <c r="J59" s="36">
+      <c r="J59" s="32">
         <v>3592.7</v>
       </c>
-      <c r="K59" s="36">
+      <c r="K59" s="32">
         <v>1379.1</v>
       </c>
-      <c r="L59" s="36">
+      <c r="L59" s="32">
         <v>2208.8000000000002</v>
       </c>
-      <c r="M59" s="36">
+      <c r="M59" s="32">
         <v>5866.1</v>
       </c>
-      <c r="N59" s="36">
+      <c r="N59" s="32">
         <v>2037.4</v>
       </c>
-      <c r="O59" s="36">
+      <c r="O59" s="32">
         <v>3828.7</v>
       </c>
-      <c r="P59" s="37">
+      <c r="P59" s="33">
         <v>355.88499999999999</v>
       </c>
-      <c r="Q59" s="37">
+      <c r="Q59" s="33">
         <v>4.5439999999999996</v>
       </c>
     </row>
@@ -26663,52 +26954,52 @@
       <c r="A60" s="1">
         <v>48121</v>
       </c>
-      <c r="B60" s="36">
+      <c r="B60" s="32">
         <v>35822</v>
       </c>
-      <c r="C60" s="36">
+      <c r="C60" s="32">
         <v>23656</v>
       </c>
-      <c r="D60" s="36">
+      <c r="D60" s="32">
         <v>23774.799999999999</v>
       </c>
-      <c r="E60" s="36">
+      <c r="E60" s="32">
         <v>35967</v>
       </c>
-      <c r="F60" s="37">
+      <c r="F60" s="33">
         <v>146.80799999999999</v>
       </c>
-      <c r="G60" s="37">
+      <c r="G60" s="33">
         <v>151.428</v>
       </c>
-      <c r="H60" s="36">
+      <c r="H60" s="32">
         <v>24540.400000000001</v>
       </c>
-      <c r="I60" s="36">
+      <c r="I60" s="32">
         <v>16716</v>
       </c>
-      <c r="J60" s="36">
+      <c r="J60" s="32">
         <v>3596.4</v>
       </c>
-      <c r="K60" s="36">
+      <c r="K60" s="32">
         <v>1379.3</v>
       </c>
-      <c r="L60" s="36">
+      <c r="L60" s="32">
         <v>2212.1</v>
       </c>
-      <c r="M60" s="36">
+      <c r="M60" s="32">
         <v>5913.9</v>
       </c>
-      <c r="N60" s="36">
+      <c r="N60" s="32">
         <v>2049.4</v>
       </c>
-      <c r="O60" s="36">
+      <c r="O60" s="32">
         <v>3864.5</v>
       </c>
-      <c r="P60" s="37">
+      <c r="P60" s="33">
         <v>357.94499999999999</v>
       </c>
-      <c r="Q60" s="37">
+      <c r="Q60" s="33">
         <v>4.5380000000000003</v>
       </c>
     </row>
@@ -26716,52 +27007,52 @@
       <c r="A61" s="1">
         <v>48213</v>
       </c>
-      <c r="B61" s="36">
+      <c r="B61" s="32">
         <v>36162.400000000001</v>
       </c>
-      <c r="C61" s="36">
+      <c r="C61" s="32">
         <v>23757.5</v>
       </c>
-      <c r="D61" s="36">
+      <c r="D61" s="32">
         <v>23876.7</v>
       </c>
-      <c r="E61" s="36">
+      <c r="E61" s="32">
         <v>36308.300000000003</v>
       </c>
-      <c r="F61" s="37">
+      <c r="F61" s="33">
         <v>147.541</v>
       </c>
-      <c r="G61" s="37">
+      <c r="G61" s="33">
         <v>152.214</v>
       </c>
-      <c r="H61" s="36">
+      <c r="H61" s="32">
         <v>24787.5</v>
       </c>
-      <c r="I61" s="36">
+      <c r="I61" s="32">
         <v>16800.400000000001</v>
       </c>
-      <c r="J61" s="36">
+      <c r="J61" s="32">
         <v>3600.1</v>
       </c>
-      <c r="K61" s="36">
+      <c r="K61" s="32">
         <v>1379.6</v>
       </c>
-      <c r="L61" s="36">
+      <c r="L61" s="32">
         <v>2215.3000000000002</v>
       </c>
-      <c r="M61" s="36">
+      <c r="M61" s="32">
         <v>5962</v>
       </c>
-      <c r="N61" s="36">
+      <c r="N61" s="32">
         <v>2061.4</v>
       </c>
-      <c r="O61" s="36">
+      <c r="O61" s="32">
         <v>3900.6</v>
       </c>
-      <c r="P61" s="37">
+      <c r="P61" s="33">
         <v>360.01299999999998</v>
       </c>
-      <c r="Q61" s="37">
+      <c r="Q61" s="33">
         <v>4.5309999999999997</v>
       </c>
     </row>
@@ -26769,52 +27060,52 @@
       <c r="A62" s="1">
         <v>48304</v>
       </c>
-      <c r="B62" s="36">
+      <c r="B62" s="32">
         <v>36505.5</v>
       </c>
-      <c r="C62" s="36">
+      <c r="C62" s="32">
         <v>23859.200000000001</v>
       </c>
-      <c r="D62" s="36">
+      <c r="D62" s="32">
         <v>23978.9</v>
       </c>
-      <c r="E62" s="36">
+      <c r="E62" s="32">
         <v>36652.300000000003</v>
       </c>
-      <c r="F62" s="37">
+      <c r="F62" s="33">
         <v>148.27699999999999</v>
       </c>
-      <c r="G62" s="37">
+      <c r="G62" s="33">
         <v>153.00299999999999</v>
       </c>
-      <c r="H62" s="36">
+      <c r="H62" s="32">
         <v>25037.8</v>
       </c>
-      <c r="I62" s="36">
+      <c r="I62" s="32">
         <v>16885.8</v>
       </c>
-      <c r="J62" s="36">
+      <c r="J62" s="32">
         <v>3603.8</v>
       </c>
-      <c r="K62" s="36">
+      <c r="K62" s="32">
         <v>1379.8</v>
       </c>
-      <c r="L62" s="36">
+      <c r="L62" s="32">
         <v>2218.6</v>
       </c>
-      <c r="M62" s="36">
+      <c r="M62" s="32">
         <v>6010.5</v>
       </c>
-      <c r="N62" s="36">
+      <c r="N62" s="32">
         <v>2073.5</v>
       </c>
-      <c r="O62" s="36">
+      <c r="O62" s="32">
         <v>3937</v>
       </c>
-      <c r="P62" s="37">
+      <c r="P62" s="33">
         <v>362.09</v>
       </c>
-      <c r="Q62" s="37">
+      <c r="Q62" s="33">
         <v>4.524</v>
       </c>
     </row>
@@ -26822,52 +27113,52 @@
       <c r="A63" s="1">
         <v>48395</v>
       </c>
-      <c r="B63" s="36">
+      <c r="B63" s="32">
         <v>36851.1</v>
       </c>
-      <c r="C63" s="36">
+      <c r="C63" s="32">
         <v>23961.1</v>
       </c>
-      <c r="D63" s="36">
+      <c r="D63" s="32">
         <v>24081.3</v>
       </c>
-      <c r="E63" s="36">
+      <c r="E63" s="32">
         <v>36998.800000000003</v>
       </c>
-      <c r="F63" s="37">
+      <c r="F63" s="33">
         <v>149.01499999999999</v>
       </c>
-      <c r="G63" s="37">
+      <c r="G63" s="33">
         <v>153.79499999999999</v>
       </c>
-      <c r="H63" s="36">
+      <c r="H63" s="32">
         <v>25289.4</v>
       </c>
-      <c r="I63" s="36">
+      <c r="I63" s="32">
         <v>16971.099999999999</v>
       </c>
-      <c r="J63" s="36">
+      <c r="J63" s="32">
         <v>3607.6</v>
       </c>
-      <c r="K63" s="36">
+      <c r="K63" s="32">
         <v>1380.1</v>
       </c>
-      <c r="L63" s="36">
+      <c r="L63" s="32">
         <v>2221.9</v>
       </c>
-      <c r="M63" s="36">
+      <c r="M63" s="32">
         <v>6059.5</v>
       </c>
-      <c r="N63" s="36">
+      <c r="N63" s="32">
         <v>2085.6999999999998</v>
       </c>
-      <c r="O63" s="36">
+      <c r="O63" s="32">
         <v>3973.8</v>
       </c>
-      <c r="P63" s="37">
+      <c r="P63" s="33">
         <v>364.17700000000002</v>
       </c>
-      <c r="Q63" s="37">
+      <c r="Q63" s="33">
         <v>4.5170000000000003</v>
       </c>
     </row>
@@ -26875,52 +27166,52 @@
       <c r="A64" s="1">
         <v>48487</v>
       </c>
-      <c r="B64" s="36">
+      <c r="B64" s="32">
         <v>37199.1</v>
       </c>
-      <c r="C64" s="36">
+      <c r="C64" s="32">
         <v>24063</v>
       </c>
-      <c r="D64" s="36">
+      <c r="D64" s="32">
         <v>24183.7</v>
       </c>
-      <c r="E64" s="36">
+      <c r="E64" s="32">
         <v>37347.699999999997</v>
       </c>
-      <c r="F64" s="37">
+      <c r="F64" s="33">
         <v>149.755</v>
       </c>
-      <c r="G64" s="37">
+      <c r="G64" s="33">
         <v>154.59</v>
       </c>
-      <c r="H64" s="36">
+      <c r="H64" s="32">
         <v>25543.3</v>
       </c>
-      <c r="I64" s="36">
+      <c r="I64" s="32">
         <v>17056.599999999999</v>
       </c>
-      <c r="J64" s="36">
+      <c r="J64" s="32">
         <v>3611.4</v>
       </c>
-      <c r="K64" s="36">
+      <c r="K64" s="32">
         <v>1380.4</v>
       </c>
-      <c r="L64" s="36">
+      <c r="L64" s="32">
         <v>2225.1999999999998</v>
       </c>
-      <c r="M64" s="36">
+      <c r="M64" s="32">
         <v>6108.9</v>
       </c>
-      <c r="N64" s="36">
+      <c r="N64" s="32">
         <v>2097.9</v>
       </c>
-      <c r="O64" s="36">
+      <c r="O64" s="32">
         <v>4010.9</v>
       </c>
-      <c r="P64" s="37">
+      <c r="P64" s="33">
         <v>366.274</v>
       </c>
-      <c r="Q64" s="37">
+      <c r="Q64" s="33">
         <v>4.51</v>
       </c>
     </row>
@@ -26928,58 +27219,58 @@
       <c r="A65" s="1">
         <v>48579</v>
       </c>
-      <c r="B65" s="36">
+      <c r="B65" s="32">
         <v>37549.5</v>
       </c>
-      <c r="C65" s="36">
+      <c r="C65" s="32">
         <v>24164.9</v>
       </c>
-      <c r="D65" s="36">
+      <c r="D65" s="32">
         <v>24286.1</v>
       </c>
-      <c r="E65" s="36">
+      <c r="E65" s="32">
         <v>37699</v>
       </c>
-      <c r="F65" s="37">
+      <c r="F65" s="33">
         <v>150.499</v>
       </c>
-      <c r="G65" s="37">
+      <c r="G65" s="33">
         <v>155.38800000000001</v>
       </c>
-      <c r="H65" s="36">
+      <c r="H65" s="32">
         <v>25797.9</v>
       </c>
-      <c r="I65" s="36">
+      <c r="I65" s="32">
         <v>17141.599999999999</v>
       </c>
-      <c r="J65" s="36">
+      <c r="J65" s="32">
         <v>3615.3</v>
       </c>
-      <c r="K65" s="36">
+      <c r="K65" s="32">
         <v>1380.8</v>
       </c>
-      <c r="L65" s="36">
+      <c r="L65" s="32">
         <v>2228.6</v>
       </c>
-      <c r="M65" s="36">
+      <c r="M65" s="32">
         <v>6158.9</v>
       </c>
-      <c r="N65" s="36">
+      <c r="N65" s="32">
         <v>2110.6</v>
       </c>
-      <c r="O65" s="36">
+      <c r="O65" s="32">
         <v>4048.4</v>
       </c>
-      <c r="P65" s="37">
+      <c r="P65" s="33">
         <v>368.38</v>
       </c>
-      <c r="Q65" s="37">
+      <c r="Q65" s="33">
         <v>4.5030000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I66" s="38"/>
-      <c r="L66" s="38"/>
+      <c r="I66" s="34"/>
+      <c r="L66" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -26988,10 +27279,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77260E8A-45C6-C74E-A071-E1E958901B15}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView zoomScale="107" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -27164,29 +27455,29 @@
       <c r="A6">
         <v>2021</v>
       </c>
-      <c r="B6" s="24">
-        <v>2675.6800560000001</v>
-      </c>
-      <c r="C6" s="25">
-        <v>1698.961</v>
-      </c>
-      <c r="D6" s="25">
-        <v>317.62599999999998</v>
-      </c>
-      <c r="E6" s="25">
-        <v>164.04599999999999</v>
-      </c>
-      <c r="F6" s="25">
-        <v>1325.337</v>
-      </c>
-      <c r="G6" s="25">
-        <v>830.23699999999997</v>
-      </c>
-      <c r="H6" s="25">
-        <v>507.26100000000002</v>
-      </c>
-      <c r="I6" s="25">
-        <v>242.08699999999999</v>
+      <c r="B6" s="43">
+        <v>3460.683</v>
+      </c>
+      <c r="C6" s="42">
+        <v>2044.377</v>
+      </c>
+      <c r="D6" s="42">
+        <v>316.81599999999997</v>
+      </c>
+      <c r="E6" s="42">
+        <v>371.83100000000002</v>
+      </c>
+      <c r="F6" s="42">
+        <v>1314.088</v>
+      </c>
+      <c r="G6" s="42">
+        <v>867.67600000000004</v>
+      </c>
+      <c r="H6" s="42">
+        <v>520.58799999999997</v>
+      </c>
+      <c r="I6" s="42">
+        <v>391.74700000000001</v>
       </c>
       <c r="J6" s="23">
         <v>59.15</v>
@@ -27196,29 +27487,29 @@
       <c r="A7">
         <v>2022</v>
       </c>
-      <c r="B7" s="24">
-        <v>2725.1688960000001</v>
-      </c>
-      <c r="C7" s="25">
-        <v>2040.5219999999999</v>
-      </c>
-      <c r="D7" s="25">
-        <v>350.88200000000001</v>
-      </c>
-      <c r="E7" s="25">
-        <v>251.98500000000001</v>
-      </c>
-      <c r="F7" s="25">
-        <v>1351.277</v>
-      </c>
-      <c r="G7" s="25">
-        <v>942.86400000000003</v>
-      </c>
-      <c r="H7" s="25">
-        <v>514.14599999999996</v>
-      </c>
-      <c r="I7" s="25">
-        <v>40.164000000000001</v>
+      <c r="B7" s="43">
+        <v>2820.0129999999999</v>
+      </c>
+      <c r="C7" s="42">
+        <v>2622.5050000000001</v>
+      </c>
+      <c r="D7" s="42">
+        <v>354.14499999999998</v>
+      </c>
+      <c r="E7" s="42">
+        <v>394.8</v>
+      </c>
+      <c r="F7" s="42">
+        <v>1464.5930000000001</v>
+      </c>
+      <c r="G7" s="42">
+        <v>941.351</v>
+      </c>
+      <c r="H7" s="42">
+        <v>589.25400000000002</v>
+      </c>
+      <c r="I7" s="42">
+        <v>39.683999999999997</v>
       </c>
       <c r="J7" s="23">
         <v>38.14</v>
@@ -27228,29 +27519,29 @@
       <c r="A8">
         <v>2023</v>
       </c>
-      <c r="B8" s="24">
-        <v>2789.7678000000001</v>
-      </c>
-      <c r="C8" s="25">
-        <v>2084.1019999999999</v>
-      </c>
-      <c r="D8" s="25">
-        <v>361.96100000000001</v>
-      </c>
-      <c r="E8" s="25">
-        <v>303.99599999999998</v>
-      </c>
-      <c r="F8" s="25">
-        <v>1452.09</v>
-      </c>
-      <c r="G8" s="25">
-        <v>1017.717</v>
-      </c>
-      <c r="H8" s="25">
-        <v>491.86900000000003</v>
-      </c>
-      <c r="I8" s="25">
-        <v>37.088999999999999</v>
+      <c r="B8" s="43">
+        <v>2797.576</v>
+      </c>
+      <c r="C8" s="42">
+        <v>2578.828</v>
+      </c>
+      <c r="D8" s="42">
+        <v>282.96600000000001</v>
+      </c>
+      <c r="E8" s="42">
+        <v>456.12900000000002</v>
+      </c>
+      <c r="F8" s="42">
+        <v>1571.68</v>
+      </c>
+      <c r="G8" s="42">
+        <v>1008.7670000000001</v>
+      </c>
+      <c r="H8" s="42">
+        <v>601.34799999999996</v>
+      </c>
+      <c r="I8" s="42">
+        <v>29.963000000000001</v>
       </c>
       <c r="J8" s="23">
         <v>36.145000000000003</v>
@@ -27260,29 +27551,29 @@
       <c r="A9">
         <v>2024</v>
       </c>
-      <c r="B9" s="24">
-        <v>2862.2467660000002</v>
-      </c>
-      <c r="C9" s="25">
-        <v>2138.5259999999998</v>
-      </c>
-      <c r="D9" s="25">
-        <v>378.53399999999999</v>
-      </c>
-      <c r="E9" s="25">
-        <v>328.43299999999999</v>
-      </c>
-      <c r="F9" s="25">
-        <v>1506.7819999999999</v>
-      </c>
-      <c r="G9" s="25">
-        <v>1047.1569999999999</v>
-      </c>
-      <c r="H9" s="25">
-        <v>503.505</v>
-      </c>
-      <c r="I9" s="25">
-        <v>36.167000000000002</v>
+      <c r="B9" s="43">
+        <v>2950.2380000000003</v>
+      </c>
+      <c r="C9" s="42">
+        <v>2541.6950000000002</v>
+      </c>
+      <c r="D9" s="42">
+        <v>279.18700000000001</v>
+      </c>
+      <c r="E9" s="42">
+        <v>478.02100000000002</v>
+      </c>
+      <c r="F9" s="42">
+        <v>1624.982</v>
+      </c>
+      <c r="G9" s="42">
+        <v>1085.711</v>
+      </c>
+      <c r="H9" s="42">
+        <v>545.42499999999995</v>
+      </c>
+      <c r="I9" s="42">
+        <v>33.764000000000003</v>
       </c>
       <c r="J9" s="23">
         <v>35.369999999999997</v>
@@ -27292,29 +27583,29 @@
       <c r="A10">
         <v>2025</v>
       </c>
-      <c r="B10" s="24">
-        <v>3076.7846719999998</v>
-      </c>
-      <c r="C10" s="25">
-        <v>2227.5610000000001</v>
-      </c>
-      <c r="D10" s="25">
-        <v>365.35899999999998</v>
-      </c>
-      <c r="E10" s="25">
-        <v>355.43400000000003</v>
-      </c>
-      <c r="F10" s="25">
-        <v>1558.3019999999999</v>
-      </c>
-      <c r="G10" s="25">
-        <v>1171.548</v>
-      </c>
-      <c r="H10" s="25">
-        <v>533.43499999999995</v>
-      </c>
-      <c r="I10" s="25">
-        <v>34.216999999999999</v>
+      <c r="B10" s="43">
+        <v>3121.6370000000002</v>
+      </c>
+      <c r="C10" s="42">
+        <v>2539.1210000000001</v>
+      </c>
+      <c r="D10" s="42">
+        <v>290.19799999999998</v>
+      </c>
+      <c r="E10" s="42">
+        <v>483.15800000000002</v>
+      </c>
+      <c r="F10" s="42">
+        <v>1669.0419999999999</v>
+      </c>
+      <c r="G10" s="42">
+        <v>1165.28</v>
+      </c>
+      <c r="H10" s="42">
+        <v>547.125</v>
+      </c>
+      <c r="I10" s="42">
+        <v>36.093000000000004</v>
       </c>
       <c r="J10" s="23">
         <v>33.424999999999997</v>
@@ -27324,29 +27615,29 @@
       <c r="A11">
         <v>2026</v>
       </c>
-      <c r="B11" s="24">
-        <v>3236.1370160000001</v>
-      </c>
-      <c r="C11" s="25">
-        <v>2479.105</v>
-      </c>
-      <c r="D11" s="25">
-        <v>353.93799999999999</v>
-      </c>
-      <c r="E11" s="25">
-        <v>365.29700000000003</v>
-      </c>
-      <c r="F11" s="25">
-        <v>1618.9469999999999</v>
-      </c>
-      <c r="G11" s="25">
-        <v>1256.192</v>
-      </c>
-      <c r="H11" s="25">
-        <v>563.24099999999999</v>
-      </c>
-      <c r="I11" s="25">
-        <v>33.183999999999997</v>
+      <c r="B11" s="43">
+        <v>3312.8409999999999</v>
+      </c>
+      <c r="C11" s="42">
+        <v>2770.9430000000002</v>
+      </c>
+      <c r="D11" s="42">
+        <v>310.27800000000002</v>
+      </c>
+      <c r="E11" s="42">
+        <v>472.99400000000003</v>
+      </c>
+      <c r="F11" s="42">
+        <v>1725.508</v>
+      </c>
+      <c r="G11" s="42">
+        <v>1262.203</v>
+      </c>
+      <c r="H11" s="42">
+        <v>577.846</v>
+      </c>
+      <c r="I11" s="42">
+        <v>38.706000000000003</v>
       </c>
       <c r="J11" s="23">
         <v>32.450000000000003</v>
@@ -27356,29 +27647,29 @@
       <c r="A12">
         <v>2027</v>
       </c>
-      <c r="B12" s="24">
-        <v>3385.882263</v>
-      </c>
-      <c r="C12" s="25">
-        <v>2697.9229999999998</v>
-      </c>
-      <c r="D12" s="25">
-        <v>365.00299999999999</v>
-      </c>
-      <c r="E12" s="25">
-        <v>360.97699999999998</v>
-      </c>
-      <c r="F12" s="25">
-        <v>1672.973</v>
-      </c>
-      <c r="G12" s="25">
-        <v>1348.1610000000001</v>
-      </c>
-      <c r="H12" s="25">
-        <v>597.41200000000003</v>
-      </c>
-      <c r="I12" s="25">
-        <v>33.901000000000003</v>
+      <c r="B12" s="43">
+        <v>3489.6079999999997</v>
+      </c>
+      <c r="C12" s="42">
+        <v>2969.5929999999998</v>
+      </c>
+      <c r="D12" s="42">
+        <v>335.54300000000001</v>
+      </c>
+      <c r="E12" s="42">
+        <v>456.85199999999998</v>
+      </c>
+      <c r="F12" s="42">
+        <v>1786.4459999999999</v>
+      </c>
+      <c r="G12" s="42">
+        <v>1360.3689999999999</v>
+      </c>
+      <c r="H12" s="42">
+        <v>607.851</v>
+      </c>
+      <c r="I12" s="42">
+        <v>40.206000000000003</v>
       </c>
       <c r="J12" s="23">
         <v>33.164999999999999</v>
@@ -27388,29 +27679,29 @@
       <c r="A13">
         <v>2028</v>
       </c>
-      <c r="B13" s="24">
-        <v>3654.9385870000001</v>
-      </c>
-      <c r="C13" s="25">
-        <v>2782.221</v>
-      </c>
-      <c r="D13" s="25">
-        <v>362.74099999999999</v>
-      </c>
-      <c r="E13" s="25">
-        <v>368.625</v>
-      </c>
-      <c r="F13" s="25">
-        <v>1729.1780000000001</v>
-      </c>
-      <c r="G13" s="25">
-        <v>1516.3989999999999</v>
-      </c>
-      <c r="H13" s="25">
-        <v>631.86</v>
-      </c>
-      <c r="I13" s="25">
-        <v>35.832000000000001</v>
+      <c r="B13" s="43">
+        <v>3698.8889999999997</v>
+      </c>
+      <c r="C13" s="42">
+        <v>3049.3029999999999</v>
+      </c>
+      <c r="D13" s="42">
+        <v>351.88</v>
+      </c>
+      <c r="E13" s="42">
+        <v>461.02300000000002</v>
+      </c>
+      <c r="F13" s="42">
+        <v>1853.4290000000001</v>
+      </c>
+      <c r="G13" s="42">
+        <v>1461.5450000000001</v>
+      </c>
+      <c r="H13" s="42">
+        <v>639.17700000000002</v>
+      </c>
+      <c r="I13" s="42">
+        <v>43.817</v>
       </c>
       <c r="J13" s="23">
         <v>35.090000000000003</v>
@@ -27420,29 +27711,29 @@
       <c r="A14">
         <v>2029</v>
       </c>
-      <c r="B14" s="24">
-        <v>3651.8353670000001</v>
-      </c>
-      <c r="C14" s="25">
-        <v>2882.0140000000001</v>
-      </c>
-      <c r="D14" s="25">
-        <v>359.91500000000002</v>
-      </c>
-      <c r="E14" s="25">
-        <v>377.49</v>
-      </c>
-      <c r="F14" s="25">
-        <v>1788.18</v>
-      </c>
-      <c r="G14" s="25">
-        <v>1475.1320000000001</v>
-      </c>
-      <c r="H14" s="25">
-        <v>667.45500000000004</v>
-      </c>
-      <c r="I14" s="25">
-        <v>37.915999999999997</v>
+      <c r="B14" s="43">
+        <v>3909.2000000000007</v>
+      </c>
+      <c r="C14" s="42">
+        <v>3169.9630000000002</v>
+      </c>
+      <c r="D14" s="42">
+        <v>370.37900000000002</v>
+      </c>
+      <c r="E14" s="42">
+        <v>470.43400000000003</v>
+      </c>
+      <c r="F14" s="42">
+        <v>1923.1959999999999</v>
+      </c>
+      <c r="G14" s="42">
+        <v>1559.3230000000001</v>
+      </c>
+      <c r="H14" s="42">
+        <v>671.87</v>
+      </c>
+      <c r="I14" s="42">
+        <v>46.652000000000001</v>
       </c>
       <c r="J14" s="23">
         <v>37.164999999999999</v>
@@ -27452,29 +27743,29 @@
       <c r="A15">
         <v>2030</v>
       </c>
-      <c r="B15" s="24">
-        <v>3932.6238069999999</v>
-      </c>
-      <c r="C15" s="25">
-        <v>2985.3470000000002</v>
-      </c>
-      <c r="D15" s="25">
-        <v>357.32900000000001</v>
-      </c>
-      <c r="E15" s="25">
-        <v>385.48599999999999</v>
-      </c>
-      <c r="F15" s="25">
-        <v>1848.9970000000001</v>
-      </c>
-      <c r="G15" s="25">
-        <v>1642.68</v>
-      </c>
-      <c r="H15" s="25">
-        <v>705.01099999999997</v>
-      </c>
-      <c r="I15" s="25">
-        <v>40.545000000000002</v>
+      <c r="B15" s="43">
+        <v>4136.3910000000005</v>
+      </c>
+      <c r="C15" s="42">
+        <v>3300.931</v>
+      </c>
+      <c r="D15" s="42">
+        <v>384.83100000000002</v>
+      </c>
+      <c r="E15" s="42">
+        <v>480.08300000000003</v>
+      </c>
+      <c r="F15" s="42">
+        <v>1995.49</v>
+      </c>
+      <c r="G15" s="42">
+        <v>1672.029</v>
+      </c>
+      <c r="H15" s="42">
+        <v>708.27200000000005</v>
+      </c>
+      <c r="I15" s="42">
+        <v>48.414000000000001</v>
       </c>
       <c r="J15" s="23">
         <v>39.784999999999997</v>
@@ -27484,33 +27775,76 @@
       <c r="A16">
         <v>2031</v>
       </c>
-      <c r="B16" s="24">
-        <v>3932.6238069999999</v>
-      </c>
-      <c r="C16" s="25">
-        <v>3096.473</v>
-      </c>
-      <c r="D16" s="25">
-        <v>367.358</v>
-      </c>
-      <c r="E16" s="25">
-        <v>392.95400000000001</v>
-      </c>
-      <c r="F16" s="25">
-        <v>1914.1849999999999</v>
-      </c>
-      <c r="G16" s="25">
-        <v>1781.768</v>
-      </c>
-      <c r="H16" s="25">
-        <v>744.03499999999997</v>
-      </c>
-      <c r="I16" s="25">
-        <v>45.503</v>
+      <c r="B16" s="43">
+        <v>4361.9230000000007</v>
+      </c>
+      <c r="C16" s="42">
+        <v>3435.5259999999998</v>
+      </c>
+      <c r="D16" s="42">
+        <v>403.47</v>
+      </c>
+      <c r="E16" s="42">
+        <v>491.02199999999999</v>
+      </c>
+      <c r="F16" s="42">
+        <v>2071.7869999999998</v>
+      </c>
+      <c r="G16" s="42">
+        <v>1782.018</v>
+      </c>
+      <c r="H16" s="42">
+        <v>748.83299999999997</v>
+      </c>
+      <c r="I16" s="42">
+        <v>50.064</v>
       </c>
       <c r="J16" s="23">
         <v>44.73</v>
       </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2032</v>
+      </c>
+      <c r="B17" s="43">
+        <v>4630.4039999999995</v>
+      </c>
+      <c r="C17" s="42">
+        <v>3582.4940000000001</v>
+      </c>
+      <c r="D17" s="42">
+        <v>424.18400000000003</v>
+      </c>
+      <c r="E17" s="42">
+        <v>505.16</v>
+      </c>
+      <c r="F17" s="42">
+        <v>2150.2310000000002</v>
+      </c>
+      <c r="G17" s="42">
+        <v>1929.3679999999999</v>
+      </c>
+      <c r="H17" s="42">
+        <v>789.40700000000004</v>
+      </c>
+      <c r="I17" s="42">
+        <v>51.475000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27521,8 +27855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DE4D24-926E-5240-89B6-F8FE59F1901D}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed forecast sheet with cbo methodology, incorporated mpi
</commit_message>
<xml_diff>
--- a/inst/extdata/projections.xlsx
+++ b/inst/extdata/projections.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsalwati\Downloads\Hutchins Fiscal Impact Measure\fim\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0D213E1-11F1-4D06-9944-E15B378E3F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F6F29A-50CE-4323-9116-95E5969FD3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="10" r:id="rId1"/>
     <sheet name="pre-pandemic economic" sheetId="9" r:id="rId2"/>
-    <sheet name="economic" sheetId="1" r:id="rId3"/>
+    <sheet name="economic" sheetId="11" r:id="rId3"/>
     <sheet name="budget" sheetId="3" r:id="rId4"/>
     <sheet name="quarterly fmap" sheetId="7" r:id="rId5"/>
     <sheet name="annual fmap" sheetId="8" r:id="rId6"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="273">
   <si>
     <t>date</t>
   </si>
@@ -724,54 +724,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>gdp, "Output", "Gross Domestic Product (GDP)", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "gdph", "Output", "Real GDP", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "gdppotq", "Potential GDP and Its Components", "Potential GDP", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "gdppothq", "Potential GDP and Its Components", "Real Potential GDP", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "dc", "Prices", "Price Index, Personal Consumption Expenditures (PCE)", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "cpiu", "Prices", "Consumer Price Index, All Urban Consumers (CPI-U)", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "jgdp", "Prices", "GDP Price Index", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "unemployment_rate", "Labor", "Unemployment Rate, Civilian, 16 Years or Older", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "c", "Components of GDP (Nominal)", "Personal Consumption Expenditures", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "g", "Components of GDP (Nominal)", "Government Consumption Expenditures and Gross Investment", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "gf", "Components of GDP (Nominal)", "Government Consumption Expenditures and Gross Investment", "Federal",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "gs", "Components of GDP (Nominal)", "Government Consumption Expenditures and Gross Investment", "State and local ",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "ch", "Components of GDP (Real)", "Personal Consumption Expenditures", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "gh", "Components of GDP (Real)", "Government Consumption Expenditures and Gross Investment", NA,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "gfh", "Components of GDP (Real)", "Government Consumption Expenditures and Gross Investment", "Federal",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "gsh", "Components of GDP (Real)", "Government Consumption Expenditures and Gross Investment", "State and local "</t>
-  </si>
-  <si>
     <t xml:space="preserve">Economic 10 yr Projection, Quarterly </t>
   </si>
   <si>
@@ -827,6 +779,120 @@
   </si>
   <si>
     <t>Revenues;Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Output"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Gross Domestic Product (GDP)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Real GDP"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Potential GDP and Its Components"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Potential GDP"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "gdppothq"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Real Potential GDP"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "dc"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Prices"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Price Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Personal Consumption Expenditures (PCE)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "cpiu"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Consumer Price Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All Urban Consumers (CPI-U)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "jgdp"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "GDP Price Index"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "unemployment_rate"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Labor"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Unemployment Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Civilian</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16 Years or Older"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "c"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Components of GDP (Nominal)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Personal Consumption Expenditures"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "g"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Government Consumption Expenditures and Gross Investment"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "gf"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Federal"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "gs"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "State and local "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "ch"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Components of GDP (Real)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "gh"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "gfh"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "gsh"</t>
+  </si>
+  <si>
+    <t>"gdph"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "gdppotq"</t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1507,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1"/>
@@ -1481,6 +1547,23 @@
     <xf numFmtId="1" fontId="19" fillId="36" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="19" fillId="36" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="46" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1491,19 +1574,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1868,289 +1938,397 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.625" customWidth="1"/>
+    <col min="1" max="1" width="25.375" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="50.375" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
+    <col min="5" max="5" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+        <v>1</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
-        <v>217</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+        <v>271</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>218</v>
-      </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+        <v>272</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
-        <v>219</v>
-      </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+        <v>241</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>220</v>
-      </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+        <v>243</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+        <v>247</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>222</v>
-      </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+        <v>250</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
-        <v>223</v>
-      </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+        <v>252</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+        <v>257</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+        <v>260</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
-        <v>226</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+        <v>262</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="39" t="s">
-        <v>227</v>
-      </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
+        <v>264</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
-        <v>228</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+        <v>266</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
-        <v>229</v>
-      </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
+        <v>268</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
+        <v>269</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
-        <v>231</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
+        <v>270</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
     </row>
     <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="B22" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B23" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="B25" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B27" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B28" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="B29" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B30" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2192,27 +2370,27 @@
       </c>
     </row>
     <row r="2" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="4" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -23050,12 +23228,12 @@
       </c>
     </row>
     <row r="130" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="38" t="s">
+      <c r="A130" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B130" s="38"/>
-      <c r="C130" s="38"/>
-      <c r="D130" s="38"/>
+      <c r="B130" s="45"/>
+      <c r="C130" s="45"/>
+      <c r="D130" s="45"/>
     </row>
     <row r="131" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C131" s="6"/>
@@ -23763,14 +23941,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35EE37A-6DA7-464E-B4F9-9D022FBE10B3}">
   <dimension ref="A1:BJ66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -27455,28 +27633,28 @@
       <c r="A6">
         <v>2021</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="37">
         <v>3460.683</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="36">
         <v>2044.377</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="36">
         <v>316.81599999999997</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="36">
         <v>371.83100000000002</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="36">
         <v>1314.088</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="36">
         <v>867.67600000000004</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="36">
         <v>520.58799999999997</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="36">
         <v>391.74700000000001</v>
       </c>
       <c r="J6" s="23">
@@ -27487,28 +27665,28 @@
       <c r="A7">
         <v>2022</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="37">
         <v>2820.0129999999999</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="36">
         <v>2622.5050000000001</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="36">
         <v>354.14499999999998</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="36">
         <v>394.8</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="36">
         <v>1464.5930000000001</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="36">
         <v>941.351</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="36">
         <v>589.25400000000002</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="36">
         <v>39.683999999999997</v>
       </c>
       <c r="J7" s="23">
@@ -27519,28 +27697,28 @@
       <c r="A8">
         <v>2023</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="37">
         <v>2797.576</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="36">
         <v>2578.828</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="36">
         <v>282.96600000000001</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="36">
         <v>456.12900000000002</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="36">
         <v>1571.68</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="36">
         <v>1008.7670000000001</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="36">
         <v>601.34799999999996</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="36">
         <v>29.963000000000001</v>
       </c>
       <c r="J8" s="23">
@@ -27551,28 +27729,28 @@
       <c r="A9">
         <v>2024</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="37">
         <v>2950.2380000000003</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="36">
         <v>2541.6950000000002</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="36">
         <v>279.18700000000001</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="36">
         <v>478.02100000000002</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="36">
         <v>1624.982</v>
       </c>
-      <c r="G9" s="42">
+      <c r="G9" s="36">
         <v>1085.711</v>
       </c>
-      <c r="H9" s="42">
+      <c r="H9" s="36">
         <v>545.42499999999995</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="36">
         <v>33.764000000000003</v>
       </c>
       <c r="J9" s="23">
@@ -27583,28 +27761,28 @@
       <c r="A10">
         <v>2025</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="37">
         <v>3121.6370000000002</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="36">
         <v>2539.1210000000001</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="36">
         <v>290.19799999999998</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="36">
         <v>483.15800000000002</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="36">
         <v>1669.0419999999999</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="36">
         <v>1165.28</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="36">
         <v>547.125</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="36">
         <v>36.093000000000004</v>
       </c>
       <c r="J10" s="23">
@@ -27615,28 +27793,28 @@
       <c r="A11">
         <v>2026</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B11" s="37">
         <v>3312.8409999999999</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="36">
         <v>2770.9430000000002</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="36">
         <v>310.27800000000002</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="36">
         <v>472.99400000000003</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="36">
         <v>1725.508</v>
       </c>
-      <c r="G11" s="42">
+      <c r="G11" s="36">
         <v>1262.203</v>
       </c>
-      <c r="H11" s="42">
+      <c r="H11" s="36">
         <v>577.846</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="36">
         <v>38.706000000000003</v>
       </c>
       <c r="J11" s="23">
@@ -27647,28 +27825,28 @@
       <c r="A12">
         <v>2027</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B12" s="37">
         <v>3489.6079999999997</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="36">
         <v>2969.5929999999998</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="36">
         <v>335.54300000000001</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="36">
         <v>456.85199999999998</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="36">
         <v>1786.4459999999999</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="36">
         <v>1360.3689999999999</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="36">
         <v>607.851</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="36">
         <v>40.206000000000003</v>
       </c>
       <c r="J12" s="23">
@@ -27679,28 +27857,28 @@
       <c r="A13">
         <v>2028</v>
       </c>
-      <c r="B13" s="43">
+      <c r="B13" s="37">
         <v>3698.8889999999997</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="36">
         <v>3049.3029999999999</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="36">
         <v>351.88</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="36">
         <v>461.02300000000002</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="36">
         <v>1853.4290000000001</v>
       </c>
-      <c r="G13" s="42">
+      <c r="G13" s="36">
         <v>1461.5450000000001</v>
       </c>
-      <c r="H13" s="42">
+      <c r="H13" s="36">
         <v>639.17700000000002</v>
       </c>
-      <c r="I13" s="42">
+      <c r="I13" s="36">
         <v>43.817</v>
       </c>
       <c r="J13" s="23">
@@ -27711,28 +27889,28 @@
       <c r="A14">
         <v>2029</v>
       </c>
-      <c r="B14" s="43">
+      <c r="B14" s="37">
         <v>3909.2000000000007</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="36">
         <v>3169.9630000000002</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="36">
         <v>370.37900000000002</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="36">
         <v>470.43400000000003</v>
       </c>
-      <c r="F14" s="42">
+      <c r="F14" s="36">
         <v>1923.1959999999999</v>
       </c>
-      <c r="G14" s="42">
+      <c r="G14" s="36">
         <v>1559.3230000000001</v>
       </c>
-      <c r="H14" s="42">
+      <c r="H14" s="36">
         <v>671.87</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I14" s="36">
         <v>46.652000000000001</v>
       </c>
       <c r="J14" s="23">
@@ -27743,28 +27921,28 @@
       <c r="A15">
         <v>2030</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B15" s="37">
         <v>4136.3910000000005</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="36">
         <v>3300.931</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="36">
         <v>384.83100000000002</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="36">
         <v>480.08300000000003</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F15" s="36">
         <v>1995.49</v>
       </c>
-      <c r="G15" s="42">
+      <c r="G15" s="36">
         <v>1672.029</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="36">
         <v>708.27200000000005</v>
       </c>
-      <c r="I15" s="42">
+      <c r="I15" s="36">
         <v>48.414000000000001</v>
       </c>
       <c r="J15" s="23">
@@ -27775,28 +27953,28 @@
       <c r="A16">
         <v>2031</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16" s="37">
         <v>4361.9230000000007</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="36">
         <v>3435.5259999999998</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="36">
         <v>403.47</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="36">
         <v>491.02199999999999</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="36">
         <v>2071.7869999999998</v>
       </c>
-      <c r="G16" s="42">
+      <c r="G16" s="36">
         <v>1782.018</v>
       </c>
-      <c r="H16" s="42">
+      <c r="H16" s="36">
         <v>748.83299999999997</v>
       </c>
-      <c r="I16" s="42">
+      <c r="I16" s="36">
         <v>50.064</v>
       </c>
       <c r="J16" s="23">
@@ -27807,44 +27985,44 @@
       <c r="A17">
         <v>2032</v>
       </c>
-      <c r="B17" s="43">
+      <c r="B17" s="37">
         <v>4630.4039999999995</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="36">
         <v>3582.4940000000001</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="36">
         <v>424.18400000000003</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="36">
         <v>505.16</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="36">
         <v>2150.2310000000002</v>
       </c>
-      <c r="G17" s="42">
+      <c r="G17" s="36">
         <v>1929.3679999999999</v>
       </c>
-      <c r="H17" s="42">
+      <c r="H17" s="36">
         <v>789.40700000000004</v>
       </c>
-      <c r="I17" s="42">
+      <c r="I17" s="36">
         <v>51.475000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27855,7 +28033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DE4D24-926E-5240-89B6-F8FE59F1901D}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added dictionary sheet to projections.xlsx
old dictionary still in workbook, called dictionary_old
</commit_message>
<xml_diff>
--- a/inst/extdata/projections.xlsx
+++ b/inst/extdata/projections.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsalwati\Downloads\Hutchins Fiscal Impact Measure\fim\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9933A1D6-CBC0-49C9-8C67-2219B20A6945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1991280A-36E7-444D-82EF-D3DD91C7546A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="dictionary" sheetId="10" r:id="rId1"/>
-    <sheet name="pre-pandemic economic" sheetId="9" r:id="rId2"/>
-    <sheet name="economic" sheetId="11" r:id="rId3"/>
-    <sheet name="budget" sheetId="3" r:id="rId4"/>
-    <sheet name="quarterly fmap" sheetId="7" r:id="rId5"/>
-    <sheet name="annual fmap" sheetId="8" r:id="rId6"/>
-    <sheet name="CARES" sheetId="6" r:id="rId7"/>
-    <sheet name="crrca" sheetId="5" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId9"/>
-    <sheet name="1. Quarterly" sheetId="2" r:id="rId10"/>
+    <sheet name="dictionary" sheetId="12" r:id="rId1"/>
+    <sheet name="economic" sheetId="11" r:id="rId2"/>
+    <sheet name="budget" sheetId="3" r:id="rId3"/>
+    <sheet name="pre-pandemic economic" sheetId="9" r:id="rId4"/>
+    <sheet name="dictionary_old" sheetId="10" r:id="rId5"/>
+    <sheet name="quarterly fmap" sheetId="7" r:id="rId6"/>
+    <sheet name="annual fmap" sheetId="8" r:id="rId7"/>
+    <sheet name="CARES" sheetId="6" r:id="rId8"/>
+    <sheet name="crrca" sheetId="5" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId10"/>
+    <sheet name="1. Quarterly" sheetId="2" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="9">'1. Quarterly'!$A$5:$AZ$135</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="9">'1. Quarterly'!$A:$D</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">'1. Quarterly'!$A$5:$AZ$135</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="10">'1. Quarterly'!$A:$D</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="318">
   <si>
     <t>date</t>
   </si>
@@ -905,6 +906,129 @@
   </si>
   <si>
     <t>Sub sub category</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>economic</t>
+  </si>
+  <si>
+    <t>10-Year Economic Projections. https://www.cbo.gov/data/budget-economic-data#4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBO release </t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>Budget 10 yr Projection. https://www.cbo.gov/data/budget-economic-data#3</t>
+  </si>
+  <si>
+    <t>Mandatory Outlays Projected in CBO's Baseline, Adjusted to Exclude Effects of Timing Shifts</t>
+  </si>
+  <si>
+    <t>Major Health Care Programs&gt; Medicaid</t>
+  </si>
+  <si>
+    <t>Major Health Care Programs&gt; Medicare</t>
+  </si>
+  <si>
+    <t>Income Security Programs&gt; Unemployment Compensation</t>
+  </si>
+  <si>
+    <t>(Social Security&gt; Subtotal) + (Major Health Care Programs&gt; Subtotal) + (Income Security Programs&gt; Subtotal) - (Major Health Care Programs&gt; Medicaid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Output&gt;Gross Domestic Product (GDP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Output&gt;Real GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Potential GDP and Its Components&gt;Potential GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Potential GDP and Its Components&gt;Real Potential GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prices&gt;Price Index Personal Consumption Expenditures (PCE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prices&gt;Consumer Price Index All Urban Consumers (CPI-U)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prices&gt;GDP Price Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Labor&gt;Unemployment Rate Civilian 16 Years or Older</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components of GDP (Nominal)&gt;Personal Consumption Expenditures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components of GDP (Nominal)&gt;Government Consumption Expenditures and Gross Investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components of GDP (Nominal)&gt;Government Consumption Expenditures and Gross Investment&gt;Federal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components of GDP (Nominal)&gt;Government Consumption Expenditures and Gross Investment&gt;State and local </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components of GDP (Real)&gt;Personal Consumption Expenditures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components of GDP (Real)&gt;Government Consumption Expenditures and Gross Investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components of GDP (Real)&gt;Government Consumption Expenditures and Gross Investment&gt;Federal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components of GDP (Real)&gt;Government Consumption Expenditures and Gross Investment&gt;State and local </t>
+  </si>
+  <si>
+    <t>CBO's Baseline Budget Projections, by Category</t>
+  </si>
+  <si>
+    <t>Revenues&gt;Individual income taxes</t>
+  </si>
+  <si>
+    <t>Revenues&gt;Payroll taxes</t>
+  </si>
+  <si>
+    <t>Revenues&gt;Corporate income taxes</t>
+  </si>
+  <si>
+    <t>Revenues&gt;Other</t>
+  </si>
+  <si>
+    <t>Update the variables in each of the sheets according the CBO baseline</t>
+  </si>
+  <si>
+    <t>You will have to transpose the columns and paste in the line items</t>
+  </si>
+  <si>
+    <t>Note that some variables are a result of the sum of multiple line items</t>
+  </si>
+  <si>
+    <t>Don't change the names of the variables in the sheets</t>
+  </si>
+  <si>
+    <t>Make sure to save, run data-raw/projections.R, commit and push changes once you're done</t>
+  </si>
+  <si>
+    <t>Variable in sheet</t>
+  </si>
+  <si>
+    <t>CBO Line item</t>
+  </si>
+  <si>
+    <t>CBO Table</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1462,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1471,6 +1595,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1526,7 +1718,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1"/>
@@ -1581,6 +1773,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1597,9 +1834,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1961,422 +2195,624 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9440D-BB32-4FF5-9B05-8B4462DE649B}">
-  <dimension ref="A1:H30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386681B1-D5EF-4F8F-85A9-C01E4CBD446B}">
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.375" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="50.375" customWidth="1"/>
-    <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="19.625" customWidth="1"/>
+    <col min="1" max="2" width="19.625" style="43" customWidth="1"/>
+    <col min="3" max="3" width="26.375" style="44" customWidth="1"/>
+    <col min="4" max="5" width="19.625" style="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+    <row r="1" spans="1:16" s="48" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+    </row>
+    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>238</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>272</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>240</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>242</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
-        <v>243</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>246</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>250</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>251</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>253</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>255</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>256</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>257</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>259</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>260</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
-        <v>262</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="D13" s="35" t="s">
-        <v>263</v>
-      </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
-        <v>264</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>265</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
-        <v>266</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>259</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>269</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>263</v>
-      </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>267</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>265</v>
-      </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-    </row>
-    <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
-        <v>226</v>
-      </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>217</v>
-      </c>
-      <c r="B22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>219</v>
-      </c>
-      <c r="B23" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>221</v>
-      </c>
-      <c r="B24" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>223</v>
-      </c>
-      <c r="B25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
-        <v>225</v>
-      </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>227</v>
-      </c>
-      <c r="B27" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>228</v>
-      </c>
-      <c r="B28" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>229</v>
-      </c>
-      <c r="B29" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>230</v>
-      </c>
-      <c r="B30" t="s">
-        <v>234</v>
+      <c r="E2" s="49" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="50"/>
+    </row>
+    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="63"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>290</v>
+      </c>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="52"/>
+    </row>
+    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="63"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>291</v>
+      </c>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="52"/>
+    </row>
+    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="63"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="52"/>
+    </row>
+    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="63"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="52"/>
+    </row>
+    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="63"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>294</v>
+      </c>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="52"/>
+    </row>
+    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="63"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="52"/>
+    </row>
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="63"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="57" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>296</v>
+      </c>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="52"/>
+    </row>
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="63"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>297</v>
+      </c>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="52"/>
+    </row>
+    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="63"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>298</v>
+      </c>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="52"/>
+    </row>
+    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="63"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>299</v>
+      </c>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="52"/>
+    </row>
+    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="63"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>300</v>
+      </c>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="52"/>
+    </row>
+    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="63"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>301</v>
+      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="52"/>
+    </row>
+    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="63"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>302</v>
+      </c>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="52"/>
+    </row>
+    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="63"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>303</v>
+      </c>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="52"/>
+    </row>
+    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="64"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="54"/>
+    </row>
+    <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="62" t="s">
+        <v>282</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>288</v>
+      </c>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="50"/>
+    </row>
+    <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="63"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>285</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="52"/>
+    </row>
+    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="63"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>286</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="52"/>
+    </row>
+    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="63"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>287</v>
+      </c>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="54"/>
+    </row>
+    <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="63"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60" t="s">
+        <v>305</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>306</v>
+      </c>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="52"/>
+    </row>
+    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="63"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>307</v>
+      </c>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="52"/>
+    </row>
+    <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="63"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="51" t="s">
+        <v>308</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="52"/>
+    </row>
+    <row r="25" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="64"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="54"/>
+    </row>
+    <row r="27" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="43" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="43" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A26:C26"/>
+  <mergeCells count="7">
+    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="C2:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="C22:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2384,6 +2820,108 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E42683-B4AF-4746-955F-5BBF64474D4E}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2021</v>
+      </c>
+      <c r="B2">
+        <f>284+80.5</f>
+        <v>364.5</v>
+      </c>
+      <c r="C2">
+        <v>164</v>
+      </c>
+      <c r="D2">
+        <v>82</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>48</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7511D70-80B4-5E47-A7B7-55F3EFCB84BC}">
   <dimension ref="A1:BL135"/>
   <sheetViews>
@@ -2411,27 +2949,27 @@
       </c>
     </row>
     <row r="2" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="4" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -23269,12 +23807,12 @@
       </c>
     </row>
     <row r="130" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="47" t="s">
+      <c r="A130" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="B130" s="47"/>
-      <c r="C130" s="47"/>
-      <c r="D130" s="47"/>
+      <c r="B130" s="70"/>
+      <c r="C130" s="70"/>
+      <c r="D130" s="70"/>
     </row>
     <row r="131" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C131" s="6"/>
@@ -23396,596 +23934,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86381FD6-3DA6-864B-ACAE-10D968FEABB3}">
-  <dimension ref="A1:C53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43921</v>
-      </c>
-      <c r="B2" s="12">
-        <v>5.3959999999999999</v>
-      </c>
-      <c r="C2" s="12">
-        <v>3.8639999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44012</v>
-      </c>
-      <c r="B3" s="12">
-        <v>2.79</v>
-      </c>
-      <c r="C3" s="12">
-        <v>3.2149999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44104</v>
-      </c>
-      <c r="B4" s="12">
-        <v>2.7240000000000002</v>
-      </c>
-      <c r="C4" s="12">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44196</v>
-      </c>
-      <c r="B5" s="12">
-        <v>2.6549999999999998</v>
-      </c>
-      <c r="C5" s="12">
-        <v>3.7440000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44286</v>
-      </c>
-      <c r="B6" s="12">
-        <v>2.7839999999999998</v>
-      </c>
-      <c r="C6" s="12">
-        <v>3.734</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>44377</v>
-      </c>
-      <c r="B7" s="12">
-        <v>2.7959999999999998</v>
-      </c>
-      <c r="C7" s="12">
-        <v>3.7170000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>44469</v>
-      </c>
-      <c r="B8" s="12">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C8" s="12">
-        <v>3.72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>44561</v>
-      </c>
-      <c r="B9" s="12">
-        <v>2.4209999999999998</v>
-      </c>
-      <c r="C9" s="12">
-        <v>3.7509999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>44651</v>
-      </c>
-      <c r="B10" s="33">
-        <v>2.298</v>
-      </c>
-      <c r="C10" s="33">
-        <v>9.2159999999999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>44742</v>
-      </c>
-      <c r="B11" s="33">
-        <v>4.2320000000000002</v>
-      </c>
-      <c r="C11" s="33">
-        <v>9.843</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>44834</v>
-      </c>
-      <c r="B12" s="33">
-        <v>4.1929999999999996</v>
-      </c>
-      <c r="C12" s="33">
-        <v>7.6760000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>44926</v>
-      </c>
-      <c r="B13" s="33">
-        <v>3.786</v>
-      </c>
-      <c r="C13" s="33">
-        <v>5.7149999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>45016</v>
-      </c>
-      <c r="B14" s="33">
-        <v>4.0339999999999998</v>
-      </c>
-      <c r="C14" s="33">
-        <v>4.9859999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>45107</v>
-      </c>
-      <c r="B15" s="33">
-        <v>3.6819999999999999</v>
-      </c>
-      <c r="C15" s="33">
-        <v>4.2220000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>45199</v>
-      </c>
-      <c r="B16" s="33">
-        <v>3.3159999999999998</v>
-      </c>
-      <c r="C16" s="33">
-        <v>3.7879999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>45291</v>
-      </c>
-      <c r="B17" s="33">
-        <v>2.9569999999999999</v>
-      </c>
-      <c r="C17" s="33">
-        <v>3.6309999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>45382</v>
-      </c>
-      <c r="B18" s="33">
-        <v>3.2949999999999999</v>
-      </c>
-      <c r="C18" s="33">
-        <v>3.5049999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>45473</v>
-      </c>
-      <c r="B19" s="33">
-        <v>3.1269999999999998</v>
-      </c>
-      <c r="C19" s="33">
-        <v>3.4809999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>45565</v>
-      </c>
-      <c r="B20" s="33">
-        <v>3.125</v>
-      </c>
-      <c r="C20" s="33">
-        <v>3.5430000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>45657</v>
-      </c>
-      <c r="B21" s="33">
-        <v>3.113</v>
-      </c>
-      <c r="C21" s="33">
-        <v>3.633</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>45747</v>
-      </c>
-      <c r="B22" s="33">
-        <v>2.5430000000000001</v>
-      </c>
-      <c r="C22" s="33">
-        <v>3.8759999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>45838</v>
-      </c>
-      <c r="B23" s="33">
-        <v>2.61</v>
-      </c>
-      <c r="C23" s="33">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>45930</v>
-      </c>
-      <c r="B24" s="33">
-        <v>2.673</v>
-      </c>
-      <c r="C24" s="33">
-        <v>4.0709999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>46022</v>
-      </c>
-      <c r="B25" s="33">
-        <v>2.7309999999999999</v>
-      </c>
-      <c r="C25" s="33">
-        <v>4.0750000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>46112</v>
-      </c>
-      <c r="B26" s="33">
-        <v>2.5009999999999999</v>
-      </c>
-      <c r="C26" s="33">
-        <v>4.032</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>46203</v>
-      </c>
-      <c r="B27" s="33">
-        <v>2.59</v>
-      </c>
-      <c r="C27" s="33">
-        <v>3.9910000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>46295</v>
-      </c>
-      <c r="B28" s="33">
-        <v>2.661</v>
-      </c>
-      <c r="C28" s="33">
-        <v>3.9529999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>46387</v>
-      </c>
-      <c r="B29" s="33">
-        <v>2.6659999999999999</v>
-      </c>
-      <c r="C29" s="33">
-        <v>3.923</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>46477</v>
-      </c>
-      <c r="B30" s="33">
-        <v>2.5910000000000002</v>
-      </c>
-      <c r="C30" s="33">
-        <v>3.8959999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>46568</v>
-      </c>
-      <c r="B31" s="33">
-        <v>2.5939999999999999</v>
-      </c>
-      <c r="C31" s="33">
-        <v>3.891</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>46660</v>
-      </c>
-      <c r="B32" s="33">
-        <v>2.5960000000000001</v>
-      </c>
-      <c r="C32" s="33">
-        <v>3.8620000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>46752</v>
-      </c>
-      <c r="B33" s="33">
-        <v>2.6150000000000002</v>
-      </c>
-      <c r="C33" s="33">
-        <v>3.8380000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>46843</v>
-      </c>
-      <c r="B34" s="33">
-        <v>2.5190000000000001</v>
-      </c>
-      <c r="C34" s="33">
-        <v>3.8039999999999998</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>46934</v>
-      </c>
-      <c r="B35" s="33">
-        <v>2.5030000000000001</v>
-      </c>
-      <c r="C35" s="33">
-        <v>3.7970000000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>47026</v>
-      </c>
-      <c r="B36" s="33">
-        <v>2.4790000000000001</v>
-      </c>
-      <c r="C36" s="33">
-        <v>3.78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>47118</v>
-      </c>
-      <c r="B37" s="33">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="C37" s="33">
-        <v>3.766</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>47208</v>
-      </c>
-      <c r="B38" s="33">
-        <v>2.4620000000000002</v>
-      </c>
-      <c r="C38" s="33">
-        <v>3.74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>47299</v>
-      </c>
-      <c r="B39" s="33">
-        <v>2.4460000000000002</v>
-      </c>
-      <c r="C39" s="33">
-        <v>3.746</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>47391</v>
-      </c>
-      <c r="B40" s="33">
-        <v>2.4380000000000002</v>
-      </c>
-      <c r="C40" s="33">
-        <v>3.7570000000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>47483</v>
-      </c>
-      <c r="B41" s="33">
-        <v>2.4380000000000002</v>
-      </c>
-      <c r="C41" s="33">
-        <v>3.7709999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>47573</v>
-      </c>
-      <c r="B42" s="33">
-        <v>2.4350000000000001</v>
-      </c>
-      <c r="C42" s="33">
-        <v>3.7749999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>47664</v>
-      </c>
-      <c r="B43" s="33">
-        <v>2.431</v>
-      </c>
-      <c r="C43" s="33">
-        <v>3.7810000000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>47756</v>
-      </c>
-      <c r="B44" s="33">
-        <v>2.4279999999999999</v>
-      </c>
-      <c r="C44" s="33">
-        <v>3.7879999999999998</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>47848</v>
-      </c>
-      <c r="B45" s="33">
-        <v>2.4239999999999999</v>
-      </c>
-      <c r="C45" s="33">
-        <v>3.7879999999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>47938</v>
-      </c>
-      <c r="B46" s="33">
-        <v>2.3719999999999999</v>
-      </c>
-      <c r="C46" s="33">
-        <v>3.8069999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>48029</v>
-      </c>
-      <c r="B47" s="33">
-        <v>2.3679999999999999</v>
-      </c>
-      <c r="C47" s="33">
-        <v>3.7909999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>48121</v>
-      </c>
-      <c r="B48" s="33">
-        <v>2.3679999999999999</v>
-      </c>
-      <c r="C48" s="33">
-        <v>3.7909999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>48213</v>
-      </c>
-      <c r="B49" s="33">
-        <v>2.3690000000000002</v>
-      </c>
-      <c r="C49" s="33">
-        <v>3.7839999999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="33">
-        <v>2.3690000000000002</v>
-      </c>
-      <c r="C50" s="33">
-        <v>3.79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="33">
-        <v>2.37</v>
-      </c>
-      <c r="C51" s="33">
-        <v>3.7909999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="33">
-        <v>2.371</v>
-      </c>
-      <c r="C52" s="33">
-        <v>3.7869999999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="33">
-        <v>2.4249999999999998</v>
-      </c>
-      <c r="C53" s="33">
-        <v>3.79</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35EE37A-6DA7-464E-B4F9-9D022FBE10B3}">
   <dimension ref="A1:AT66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -24007,16 +23959,16 @@
       <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="42" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="41" t="s">
@@ -24043,10 +23995,10 @@
       <c r="O1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="42" t="s">
         <v>212</v>
       </c>
     </row>
@@ -27481,7 +27433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77260E8A-45C6-C74E-A071-E1E958901B15}">
   <dimension ref="A1:M24"/>
   <sheetViews>
@@ -28055,7 +28007,1016 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86381FD6-3DA6-864B-ACAE-10D968FEABB3}">
+  <dimension ref="A1:C53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B2" s="12">
+        <v>5.3959999999999999</v>
+      </c>
+      <c r="C2" s="12">
+        <v>3.8639999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44012</v>
+      </c>
+      <c r="B3" s="12">
+        <v>2.79</v>
+      </c>
+      <c r="C3" s="12">
+        <v>3.2149999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44104</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2.7240000000000002</v>
+      </c>
+      <c r="C4" s="12">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44196</v>
+      </c>
+      <c r="B5" s="12">
+        <v>2.6549999999999998</v>
+      </c>
+      <c r="C5" s="12">
+        <v>3.7440000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44286</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2.7839999999999998</v>
+      </c>
+      <c r="C6" s="12">
+        <v>3.734</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44377</v>
+      </c>
+      <c r="B7" s="12">
+        <v>2.7959999999999998</v>
+      </c>
+      <c r="C7" s="12">
+        <v>3.7170000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44469</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2.7669999999999999</v>
+      </c>
+      <c r="C8" s="12">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44561</v>
+      </c>
+      <c r="B9" s="12">
+        <v>2.4209999999999998</v>
+      </c>
+      <c r="C9" s="12">
+        <v>3.7509999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44651</v>
+      </c>
+      <c r="B10" s="33">
+        <v>2.298</v>
+      </c>
+      <c r="C10" s="33">
+        <v>9.2159999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44742</v>
+      </c>
+      <c r="B11" s="33">
+        <v>4.2320000000000002</v>
+      </c>
+      <c r="C11" s="33">
+        <v>9.843</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44834</v>
+      </c>
+      <c r="B12" s="33">
+        <v>4.1929999999999996</v>
+      </c>
+      <c r="C12" s="33">
+        <v>7.6760000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B13" s="33">
+        <v>3.786</v>
+      </c>
+      <c r="C13" s="33">
+        <v>5.7149999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B14" s="33">
+        <v>4.0339999999999998</v>
+      </c>
+      <c r="C14" s="33">
+        <v>4.9859999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B15" s="33">
+        <v>3.6819999999999999</v>
+      </c>
+      <c r="C15" s="33">
+        <v>4.2220000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45199</v>
+      </c>
+      <c r="B16" s="33">
+        <v>3.3159999999999998</v>
+      </c>
+      <c r="C16" s="33">
+        <v>3.7879999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45291</v>
+      </c>
+      <c r="B17" s="33">
+        <v>2.9569999999999999</v>
+      </c>
+      <c r="C17" s="33">
+        <v>3.6309999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B18" s="33">
+        <v>3.2949999999999999</v>
+      </c>
+      <c r="C18" s="33">
+        <v>3.5049999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45473</v>
+      </c>
+      <c r="B19" s="33">
+        <v>3.1269999999999998</v>
+      </c>
+      <c r="C19" s="33">
+        <v>3.4809999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45565</v>
+      </c>
+      <c r="B20" s="33">
+        <v>3.125</v>
+      </c>
+      <c r="C20" s="33">
+        <v>3.5430000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45657</v>
+      </c>
+      <c r="B21" s="33">
+        <v>3.113</v>
+      </c>
+      <c r="C21" s="33">
+        <v>3.633</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45747</v>
+      </c>
+      <c r="B22" s="33">
+        <v>2.5430000000000001</v>
+      </c>
+      <c r="C22" s="33">
+        <v>3.8759999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B23" s="33">
+        <v>2.61</v>
+      </c>
+      <c r="C23" s="33">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B24" s="33">
+        <v>2.673</v>
+      </c>
+      <c r="C24" s="33">
+        <v>4.0709999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>46022</v>
+      </c>
+      <c r="B25" s="33">
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="C25" s="33">
+        <v>4.0750000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>46112</v>
+      </c>
+      <c r="B26" s="33">
+        <v>2.5009999999999999</v>
+      </c>
+      <c r="C26" s="33">
+        <v>4.032</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>46203</v>
+      </c>
+      <c r="B27" s="33">
+        <v>2.59</v>
+      </c>
+      <c r="C27" s="33">
+        <v>3.9910000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>46295</v>
+      </c>
+      <c r="B28" s="33">
+        <v>2.661</v>
+      </c>
+      <c r="C28" s="33">
+        <v>3.9529999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>46387</v>
+      </c>
+      <c r="B29" s="33">
+        <v>2.6659999999999999</v>
+      </c>
+      <c r="C29" s="33">
+        <v>3.923</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>46477</v>
+      </c>
+      <c r="B30" s="33">
+        <v>2.5910000000000002</v>
+      </c>
+      <c r="C30" s="33">
+        <v>3.8959999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>46568</v>
+      </c>
+      <c r="B31" s="33">
+        <v>2.5939999999999999</v>
+      </c>
+      <c r="C31" s="33">
+        <v>3.891</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>46660</v>
+      </c>
+      <c r="B32" s="33">
+        <v>2.5960000000000001</v>
+      </c>
+      <c r="C32" s="33">
+        <v>3.8620000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>46752</v>
+      </c>
+      <c r="B33" s="33">
+        <v>2.6150000000000002</v>
+      </c>
+      <c r="C33" s="33">
+        <v>3.8380000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>46843</v>
+      </c>
+      <c r="B34" s="33">
+        <v>2.5190000000000001</v>
+      </c>
+      <c r="C34" s="33">
+        <v>3.8039999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>46934</v>
+      </c>
+      <c r="B35" s="33">
+        <v>2.5030000000000001</v>
+      </c>
+      <c r="C35" s="33">
+        <v>3.7970000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>47026</v>
+      </c>
+      <c r="B36" s="33">
+        <v>2.4790000000000001</v>
+      </c>
+      <c r="C36" s="33">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>47118</v>
+      </c>
+      <c r="B37" s="33">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="C37" s="33">
+        <v>3.766</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>47208</v>
+      </c>
+      <c r="B38" s="33">
+        <v>2.4620000000000002</v>
+      </c>
+      <c r="C38" s="33">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>47299</v>
+      </c>
+      <c r="B39" s="33">
+        <v>2.4460000000000002</v>
+      </c>
+      <c r="C39" s="33">
+        <v>3.746</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>47391</v>
+      </c>
+      <c r="B40" s="33">
+        <v>2.4380000000000002</v>
+      </c>
+      <c r="C40" s="33">
+        <v>3.7570000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>47483</v>
+      </c>
+      <c r="B41" s="33">
+        <v>2.4380000000000002</v>
+      </c>
+      <c r="C41" s="33">
+        <v>3.7709999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>47573</v>
+      </c>
+      <c r="B42" s="33">
+        <v>2.4350000000000001</v>
+      </c>
+      <c r="C42" s="33">
+        <v>3.7749999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>47664</v>
+      </c>
+      <c r="B43" s="33">
+        <v>2.431</v>
+      </c>
+      <c r="C43" s="33">
+        <v>3.7810000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>47756</v>
+      </c>
+      <c r="B44" s="33">
+        <v>2.4279999999999999</v>
+      </c>
+      <c r="C44" s="33">
+        <v>3.7879999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>47848</v>
+      </c>
+      <c r="B45" s="33">
+        <v>2.4239999999999999</v>
+      </c>
+      <c r="C45" s="33">
+        <v>3.7879999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>47938</v>
+      </c>
+      <c r="B46" s="33">
+        <v>2.3719999999999999</v>
+      </c>
+      <c r="C46" s="33">
+        <v>3.8069999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>48029</v>
+      </c>
+      <c r="B47" s="33">
+        <v>2.3679999999999999</v>
+      </c>
+      <c r="C47" s="33">
+        <v>3.7909999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>48121</v>
+      </c>
+      <c r="B48" s="33">
+        <v>2.3679999999999999</v>
+      </c>
+      <c r="C48" s="33">
+        <v>3.7909999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>48213</v>
+      </c>
+      <c r="B49" s="33">
+        <v>2.3690000000000002</v>
+      </c>
+      <c r="C49" s="33">
+        <v>3.7839999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="33">
+        <v>2.3690000000000002</v>
+      </c>
+      <c r="C50" s="33">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="33">
+        <v>2.37</v>
+      </c>
+      <c r="C51" s="33">
+        <v>3.7909999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="33">
+        <v>2.371</v>
+      </c>
+      <c r="C52" s="33">
+        <v>3.7869999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="33">
+        <v>2.4249999999999998</v>
+      </c>
+      <c r="C53" s="33">
+        <v>3.79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9440D-BB32-4FF5-9B05-8B4462DE649B}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.375" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="50.375" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
+    <col min="5" max="5" width="19.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+    </row>
+    <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="66" t="s">
+        <v>226</v>
+      </c>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="66" t="s">
+        <v>225</v>
+      </c>
+      <c r="B26" s="66"/>
+      <c r="C26" s="66"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>228</v>
+      </c>
+      <c r="B28" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>230</v>
+      </c>
+      <c r="B30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A26:C26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DE4D24-926E-5240-89B6-F8FE59F1901D}">
   <dimension ref="A1:J27"/>
   <sheetViews>
@@ -28289,7 +29250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B036E1FF-8773-7847-8D8D-5866CBDF4EC4}">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -28432,7 +29393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE6E772-7745-4345-AD59-C84EFCAA345D}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -28677,7 +29638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46AA86B-2BB2-174B-844E-5456E2801ADC}">
   <dimension ref="A1:O12"/>
   <sheetViews>
@@ -29202,106 +30163,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E42683-B4AF-4746-955F-5BBF64474D4E}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" t="s">
-        <v>172</v>
-      </c>
-      <c r="H1" t="s">
-        <v>178</v>
-      </c>
-      <c r="I1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" t="s">
-        <v>176</v>
-      </c>
-      <c r="K1" t="s">
-        <v>169</v>
-      </c>
-      <c r="L1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
-      </c>
-      <c r="B2">
-        <f>284+80.5</f>
-        <v>364.5</v>
-      </c>
-      <c r="C2">
-        <v>164</v>
-      </c>
-      <c r="D2">
-        <v>82</v>
-      </c>
-      <c r="E2">
-        <v>16</v>
-      </c>
-      <c r="F2">
-        <v>29</v>
-      </c>
-      <c r="G2">
-        <v>25</v>
-      </c>
-      <c r="H2">
-        <v>48</v>
-      </c>
-      <c r="I2">
-        <v>20</v>
-      </c>
-      <c r="J2">
-        <v>13</v>
-      </c>
-      <c r="K2">
-        <v>13</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2023</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
data: fix error in potential and real gdp
</commit_message>
<xml_diff>
--- a/inst/extdata/projections.xlsx
+++ b/inst/extdata/projections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\fim\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\FIM\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADC3AE3-FE13-492C-9EC7-F6396A6F98DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E7686F-B433-4EE2-AC8B-B51F732A651D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3390" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="12" r:id="rId1"/>
@@ -3440,8 +3440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386681B1-D5EF-4F8F-85A9-C01E4CBD446B}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25191,11 +25191,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35EE37A-6DA7-464E-B4F9-9D022FBE10B3}">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -25267,10 +25267,10 @@
         <v>20990.5</v>
       </c>
       <c r="D2" s="11">
+        <v>21254.6</v>
+      </c>
+      <c r="E2" s="11">
         <v>22884.6</v>
-      </c>
-      <c r="E2" s="11">
-        <v>21254.6</v>
       </c>
       <c r="F2" s="5">
         <v>106.578</v>
@@ -25320,10 +25320,10 @@
         <v>21309.5</v>
       </c>
       <c r="D3" s="11">
+        <v>21355.9</v>
+      </c>
+      <c r="E3" s="11">
         <v>23343.1</v>
-      </c>
-      <c r="E3" s="11">
-        <v>21355.9</v>
       </c>
       <c r="F3" s="5">
         <v>108.208</v>
@@ -25373,10 +25373,10 @@
         <v>21483.1</v>
       </c>
       <c r="D4" s="11">
+        <v>21461</v>
+      </c>
+      <c r="E4" s="11">
         <v>23804.5</v>
-      </c>
-      <c r="E4" s="11">
-        <v>21461</v>
       </c>
       <c r="F4" s="5">
         <v>109.705</v>
@@ -25426,10 +25426,10 @@
         <v>21847.599999999999</v>
       </c>
       <c r="D5" s="11">
+        <v>21567.1</v>
+      </c>
+      <c r="E5" s="11">
         <v>24338.1</v>
-      </c>
-      <c r="E5" s="11">
-        <v>21567.1</v>
       </c>
       <c r="F5" s="5">
         <v>111.514</v>
@@ -25479,10 +25479,10 @@
         <v>21738.9</v>
       </c>
       <c r="D6" s="11">
+        <v>21674</v>
+      </c>
+      <c r="E6" s="11">
         <v>24954.400000000001</v>
-      </c>
-      <c r="E6" s="11">
-        <v>21674</v>
       </c>
       <c r="F6" s="5">
         <v>113.59</v>
@@ -25532,10 +25532,10 @@
         <v>21708.2</v>
       </c>
       <c r="D7" s="11">
+        <v>21782</v>
+      </c>
+      <c r="E7" s="11">
         <v>25631.200000000001</v>
-      </c>
-      <c r="E7" s="11">
-        <v>21782</v>
       </c>
       <c r="F7" s="5">
         <v>115.577</v>
@@ -25585,10 +25585,10 @@
         <v>21851.1</v>
       </c>
       <c r="D8" s="11">
+        <v>21894.2</v>
+      </c>
+      <c r="E8" s="11">
         <v>26045.9</v>
-      </c>
-      <c r="E8" s="11">
-        <v>21894.2</v>
       </c>
       <c r="F8" s="5">
         <v>116.905</v>
@@ -25639,10 +25639,10 @@
         <v>21990</v>
       </c>
       <c r="D9" s="11">
+        <v>22006.9</v>
+      </c>
+      <c r="E9" s="11">
         <v>26428.7</v>
-      </c>
-      <c r="E9" s="11">
-        <v>22006.9</v>
       </c>
       <c r="F9" s="5">
         <v>118.098</v>
@@ -25692,10 +25692,10 @@
         <v>22112.3</v>
       </c>
       <c r="D10" s="11">
+        <v>22125.8</v>
+      </c>
+      <c r="E10" s="11">
         <v>26830</v>
-      </c>
-      <c r="E10" s="11">
-        <v>22125.8</v>
       </c>
       <c r="F10" s="5">
         <v>119.309</v>
@@ -25745,10 +25745,10 @@
         <v>22225.4</v>
       </c>
       <c r="D11" s="11">
+        <v>22246.2</v>
+      </c>
+      <c r="E11" s="11">
         <v>27088.400000000001</v>
-      </c>
-      <c r="E11" s="11">
-        <v>22246.2</v>
       </c>
       <c r="F11" s="5">
         <v>120.044</v>
@@ -25798,10 +25798,10 @@
         <v>22506.400000000001</v>
       </c>
       <c r="D12" s="11">
+        <v>22369.7</v>
+      </c>
+      <c r="E12" s="11">
         <v>27476.6</v>
-      </c>
-      <c r="E12" s="11">
-        <v>22369.7</v>
       </c>
       <c r="F12" s="5">
         <v>120.88</v>
@@ -25851,10 +25851,10 @@
         <v>22549.599999999999</v>
       </c>
       <c r="D13" s="53">
+        <v>22495.200000000001</v>
+      </c>
+      <c r="E13" s="53">
         <v>27775.200000000001</v>
-      </c>
-      <c r="E13" s="53">
-        <v>22495.200000000001</v>
       </c>
       <c r="F13" s="54">
         <v>121.55</v>
@@ -25904,10 +25904,10 @@
         <v>22625</v>
       </c>
       <c r="D14" s="53">
+        <v>22618.2</v>
+      </c>
+      <c r="E14" s="53">
         <v>28036.2</v>
-      </c>
-      <c r="E14" s="53">
-        <v>22618.2</v>
       </c>
       <c r="F14" s="54">
         <v>122.10899999999999</v>
@@ -25957,10 +25957,10 @@
         <v>22703.200000000001</v>
       </c>
       <c r="D15" s="53">
+        <v>22739</v>
+      </c>
+      <c r="E15" s="53">
         <v>28324.3</v>
-      </c>
-      <c r="E15" s="53">
-        <v>22739</v>
       </c>
       <c r="F15" s="54">
         <v>122.753</v>
@@ -26010,10 +26010,10 @@
         <v>22797</v>
       </c>
       <c r="D16" s="53">
+        <v>22862.7</v>
+      </c>
+      <c r="E16" s="53">
         <v>28622</v>
-      </c>
-      <c r="E16" s="53">
-        <v>22862.7</v>
       </c>
       <c r="F16" s="54">
         <v>123.42700000000001</v>
@@ -26063,10 +26063,10 @@
         <v>22895.599999999999</v>
       </c>
       <c r="D17" s="53">
+        <v>22988.799999999999</v>
+      </c>
+      <c r="E17" s="53">
         <v>28925.1</v>
-      </c>
-      <c r="E17" s="53">
-        <v>22988.799999999999</v>
       </c>
       <c r="F17" s="54">
         <v>124.102</v>
@@ -26116,10 +26116,10 @@
         <v>23007.3</v>
       </c>
       <c r="D18" s="53">
+        <v>23116.6</v>
+      </c>
+      <c r="E18" s="53">
         <v>29233.200000000001</v>
-      </c>
-      <c r="E18" s="53">
-        <v>23116.6</v>
       </c>
       <c r="F18" s="54">
         <v>124.792</v>
@@ -26169,10 +26169,10 @@
         <v>23135.599999999999</v>
       </c>
       <c r="D19" s="53">
+        <v>23245.599999999999</v>
+      </c>
+      <c r="E19" s="53">
         <v>29544.3</v>
-      </c>
-      <c r="E19" s="53">
-        <v>23245.599999999999</v>
       </c>
       <c r="F19" s="54">
         <v>125.47799999999999</v>
@@ -26222,10 +26222,10 @@
         <v>23266.6</v>
       </c>
       <c r="D20" s="53">
+        <v>23375.8</v>
+      </c>
+      <c r="E20" s="53">
         <v>29857.599999999999</v>
-      </c>
-      <c r="E20" s="53">
-        <v>23375.8</v>
       </c>
       <c r="F20" s="54">
         <v>126.16</v>
@@ -26275,10 +26275,10 @@
         <v>23405.4</v>
       </c>
       <c r="D21" s="53">
+        <v>23506.6</v>
+      </c>
+      <c r="E21" s="53">
         <v>30172.1</v>
-      </c>
-      <c r="E21" s="53">
-        <v>23506.6</v>
       </c>
       <c r="F21" s="54">
         <v>126.834</v>
@@ -26328,10 +26328,10 @@
         <v>23530.6</v>
       </c>
       <c r="D22" s="53">
+        <v>23637.9</v>
+      </c>
+      <c r="E22" s="53">
         <v>30486.7</v>
-      </c>
-      <c r="E22" s="53">
-        <v>23637.9</v>
       </c>
       <c r="F22" s="54">
         <v>127.498</v>
@@ -26381,10 +26381,10 @@
         <v>23656.9</v>
       </c>
       <c r="D23" s="53">
+        <v>23768.400000000001</v>
+      </c>
+      <c r="E23" s="53">
         <v>30801.200000000001</v>
-      </c>
-      <c r="E23" s="53">
-        <v>23768.400000000001</v>
       </c>
       <c r="F23" s="54">
         <v>128.15299999999999</v>
@@ -26434,10 +26434,10 @@
         <v>23783.200000000001</v>
       </c>
       <c r="D24" s="53">
+        <v>23898.7</v>
+      </c>
+      <c r="E24" s="53">
         <v>31117.5</v>
-      </c>
-      <c r="E24" s="53">
-        <v>23898.7</v>
       </c>
       <c r="F24" s="54">
         <v>128.803</v>
@@ -26487,10 +26487,10 @@
         <v>23909.1</v>
       </c>
       <c r="D25" s="53">
+        <v>24028.6</v>
+      </c>
+      <c r="E25" s="53">
         <v>31435</v>
-      </c>
-      <c r="E25" s="53">
-        <v>24028.6</v>
       </c>
       <c r="F25" s="54">
         <v>129.44999999999999</v>
@@ -26540,10 +26540,10 @@
         <v>24038.6</v>
       </c>
       <c r="D26" s="53">
+        <v>24159.4</v>
+      </c>
+      <c r="E26" s="53">
         <v>31755.1</v>
-      </c>
-      <c r="E26" s="53">
-        <v>24159.4</v>
       </c>
       <c r="F26" s="54">
         <v>130.095</v>
@@ -26593,10 +26593,10 @@
         <v>24166.7</v>
       </c>
       <c r="D27" s="53">
+        <v>24288.1</v>
+      </c>
+      <c r="E27" s="53">
         <v>32074.400000000001</v>
-      </c>
-      <c r="E27" s="53">
-        <v>24288.1</v>
       </c>
       <c r="F27" s="54">
         <v>130.739</v>
@@ -26646,10 +26646,10 @@
         <v>24294.3</v>
       </c>
       <c r="D28" s="53">
+        <v>24416.400000000001</v>
+      </c>
+      <c r="E28" s="53">
         <v>32395.7</v>
-      </c>
-      <c r="E28" s="53">
-        <v>24416.400000000001</v>
       </c>
       <c r="F28" s="54">
         <v>131.38300000000001</v>
@@ -26699,10 +26699,10 @@
         <v>24421.200000000001</v>
       </c>
       <c r="D29" s="53">
+        <v>24543.9</v>
+      </c>
+      <c r="E29" s="53">
         <v>32718.9</v>
-      </c>
-      <c r="E29" s="53">
-        <v>24543.9</v>
       </c>
       <c r="F29" s="54">
         <v>132.02799999999999</v>
@@ -26752,10 +26752,10 @@
         <v>24547.1</v>
       </c>
       <c r="D30" s="53">
+        <v>24670.400000000001</v>
+      </c>
+      <c r="E30" s="53">
         <v>33042.9</v>
-      </c>
-      <c r="E30" s="53">
-        <v>24670.400000000001</v>
       </c>
       <c r="F30" s="54">
         <v>132.673</v>
@@ -26805,10 +26805,10 @@
         <v>24674.6</v>
       </c>
       <c r="D31" s="53">
+        <v>24798.6</v>
+      </c>
+      <c r="E31" s="53">
         <v>33371.599999999999</v>
-      </c>
-      <c r="E31" s="53">
-        <v>24798.6</v>
       </c>
       <c r="F31" s="54">
         <v>133.31899999999999</v>
@@ -26858,10 +26858,10 @@
         <v>24802.2</v>
       </c>
       <c r="D32" s="53">
+        <v>24926.799999999999</v>
+      </c>
+      <c r="E32" s="53">
         <v>33703.300000000003</v>
-      </c>
-      <c r="E32" s="53">
-        <v>24926.799999999999</v>
       </c>
       <c r="F32" s="54">
         <v>133.96700000000001</v>
@@ -26911,10 +26911,10 @@
         <v>24930.3</v>
       </c>
       <c r="D33" s="53">
+        <v>25055.5</v>
+      </c>
+      <c r="E33" s="53">
         <v>34038.6</v>
-      </c>
-      <c r="E33" s="53">
-        <v>25055.5</v>
       </c>
       <c r="F33" s="54">
         <v>134.61699999999999</v>
@@ -26964,10 +26964,10 @@
         <v>25058</v>
       </c>
       <c r="D34" s="53">
+        <v>25183.9</v>
+      </c>
+      <c r="E34" s="53">
         <v>34376</v>
-      </c>
-      <c r="E34" s="53">
-        <v>25183.9</v>
       </c>
       <c r="F34" s="54">
         <v>135.268</v>
@@ -27017,10 +27017,10 @@
         <v>25186.2</v>
       </c>
       <c r="D35" s="53">
+        <v>25312.799999999999</v>
+      </c>
+      <c r="E35" s="53">
         <v>34716.5</v>
-      </c>
-      <c r="E35" s="53">
-        <v>25312.799999999999</v>
       </c>
       <c r="F35" s="54">
         <v>135.92099999999999</v>
@@ -27070,10 +27070,10 @@
         <v>25314.1</v>
       </c>
       <c r="D36" s="53">
+        <v>25441.3</v>
+      </c>
+      <c r="E36" s="53">
         <v>35058.800000000003</v>
-      </c>
-      <c r="E36" s="53">
-        <v>25441.3</v>
       </c>
       <c r="F36" s="54">
         <v>136.57300000000001</v>
@@ -27123,10 +27123,10 @@
         <v>25441.4</v>
       </c>
       <c r="D37" s="53">
+        <v>25569.200000000001</v>
+      </c>
+      <c r="E37" s="53">
         <v>35403.199999999997</v>
-      </c>
-      <c r="E37" s="53">
-        <v>25569.200000000001</v>
       </c>
       <c r="F37" s="54">
         <v>137.227</v>
@@ -27176,10 +27176,10 @@
         <v>25568.2</v>
       </c>
       <c r="D38" s="53">
+        <v>25696.7</v>
+      </c>
+      <c r="E38" s="53">
         <v>35749.599999999999</v>
-      </c>
-      <c r="E38" s="53">
-        <v>25696.7</v>
       </c>
       <c r="F38" s="54">
         <v>137.88499999999999</v>
@@ -27229,10 +27229,10 @@
         <v>25694.6</v>
       </c>
       <c r="D39" s="53">
+        <v>25823.8</v>
+      </c>
+      <c r="E39" s="53">
         <v>36098.6</v>
-      </c>
-      <c r="E39" s="53">
-        <v>25823.8</v>
       </c>
       <c r="F39" s="54">
         <v>138.547</v>
@@ -27282,10 +27282,10 @@
         <v>25821.1</v>
       </c>
       <c r="D40" s="53">
+        <v>25950.799999999999</v>
+      </c>
+      <c r="E40" s="53">
         <v>36450.6</v>
-      </c>
-      <c r="E40" s="53">
-        <v>25950.799999999999</v>
       </c>
       <c r="F40" s="54">
         <v>139.21199999999999</v>
@@ -27335,10 +27335,10 @@
         <v>25947.1</v>
       </c>
       <c r="D41" s="53">
+        <v>26077.5</v>
+      </c>
+      <c r="E41" s="53">
         <v>36804.9</v>
-      </c>
-      <c r="E41" s="53">
-        <v>26077.5</v>
       </c>
       <c r="F41" s="54">
         <v>139.881</v>
@@ -27388,10 +27388,10 @@
         <v>26073.200000000001</v>
       </c>
       <c r="D42" s="53">
+        <v>26204.2</v>
+      </c>
+      <c r="E42" s="53">
         <v>37162.1</v>
-      </c>
-      <c r="E42" s="53">
-        <v>26204.2</v>
       </c>
       <c r="F42" s="54">
         <v>140.553</v>
@@ -27441,10 +27441,10 @@
         <v>26199</v>
       </c>
       <c r="D43" s="53">
+        <v>26330.7</v>
+      </c>
+      <c r="E43" s="53">
         <v>37521.800000000003</v>
-      </c>
-      <c r="E43" s="53">
-        <v>26330.7</v>
       </c>
       <c r="F43" s="54">
         <v>141.22800000000001</v>
@@ -27494,10 +27494,10 @@
         <v>26325</v>
       </c>
       <c r="D44" s="53">
+        <v>26457.3</v>
+      </c>
+      <c r="E44" s="53">
         <v>37884.400000000001</v>
-      </c>
-      <c r="E44" s="53">
-        <v>26457.3</v>
       </c>
       <c r="F44" s="54">
         <v>141.90600000000001</v>
@@ -27547,10 +27547,10 @@
         <v>26450.799999999999</v>
       </c>
       <c r="D45" s="53">
+        <v>26583.7</v>
+      </c>
+      <c r="E45" s="53">
         <v>38249.300000000003</v>
-      </c>
-      <c r="E45" s="53">
-        <v>26583.7</v>
       </c>
       <c r="F45" s="54">
         <v>142.58799999999999</v>
@@ -27600,10 +27600,10 @@
         <v>26576.400000000001</v>
       </c>
       <c r="D46" s="53">
+        <v>26710</v>
+      </c>
+      <c r="E46" s="53">
         <v>38616.9</v>
-      </c>
-      <c r="E46" s="53">
-        <v>26710</v>
       </c>
       <c r="F46" s="54">
         <v>143.274</v>
@@ -27653,10 +27653,10 @@
         <v>26701.7</v>
       </c>
       <c r="D47" s="53">
+        <v>26835.9</v>
+      </c>
+      <c r="E47" s="53">
         <v>38987.1</v>
-      </c>
-      <c r="E47" s="53">
-        <v>26835.9</v>
       </c>
       <c r="F47" s="54">
         <v>143.96299999999999</v>
@@ -27706,10 +27706,10 @@
         <v>26826.799999999999</v>
       </c>
       <c r="D48" s="53">
+        <v>26961.599999999999</v>
+      </c>
+      <c r="E48" s="53">
         <v>39360.300000000003</v>
-      </c>
-      <c r="E48" s="53">
-        <v>26961.599999999999</v>
       </c>
       <c r="F48" s="54">
         <v>144.655</v>
@@ -27759,10 +27759,10 @@
         <v>26951.9</v>
       </c>
       <c r="D49" s="53">
+        <v>27087.3</v>
+      </c>
+      <c r="E49" s="53">
         <v>39736.699999999997</v>
-      </c>
-      <c r="E49" s="53">
-        <v>27087.3</v>
       </c>
       <c r="F49" s="54">
         <v>145.351</v>
@@ -27812,10 +27812,10 @@
         <v>27076.7</v>
       </c>
       <c r="D50" s="53">
+        <v>27212.799999999999</v>
+      </c>
+      <c r="E50" s="53">
         <v>40115.800000000003</v>
-      </c>
-      <c r="E50" s="53">
-        <v>27212.799999999999</v>
       </c>
       <c r="F50" s="54">
         <v>146.05000000000001</v>
@@ -27865,10 +27865,10 @@
         <v>27201.599999999999</v>
       </c>
       <c r="D51" s="53">
+        <v>27338.2</v>
+      </c>
+      <c r="E51" s="53">
         <v>40497.599999999999</v>
-      </c>
-      <c r="E51" s="53">
-        <v>27338.2</v>
       </c>
       <c r="F51" s="54">
         <v>146.75299999999999</v>
@@ -27918,10 +27918,10 @@
         <v>27326</v>
       </c>
       <c r="D52" s="53">
+        <v>27463.3</v>
+      </c>
+      <c r="E52" s="53">
         <v>40881.9</v>
-      </c>
-      <c r="E52" s="53">
-        <v>27463.3</v>
       </c>
       <c r="F52" s="54">
         <v>147.459</v>
@@ -27971,10 +27971,10 @@
         <v>27450.3</v>
       </c>
       <c r="D53" s="53">
+        <v>27588.3</v>
+      </c>
+      <c r="E53" s="53">
         <v>41268.9</v>
-      </c>
-      <c r="E53" s="53">
-        <v>27588.3</v>
       </c>
       <c r="F53" s="54">
         <v>148.16800000000001</v>
@@ -28024,10 +28024,10 @@
         <v>27574.1</v>
       </c>
       <c r="D54" s="53">
+        <v>27712.7</v>
+      </c>
+      <c r="E54" s="53">
         <v>41657.699999999997</v>
-      </c>
-      <c r="E54" s="53">
-        <v>27712.7</v>
       </c>
       <c r="F54" s="54">
         <v>148.88200000000001</v>
@@ -28077,10 +28077,10 @@
         <v>27698</v>
       </c>
       <c r="D55" s="53">
+        <v>27837.200000000001</v>
+      </c>
+      <c r="E55" s="53">
         <v>42049.7</v>
-      </c>
-      <c r="E55" s="53">
-        <v>27837.200000000001</v>
       </c>
       <c r="F55" s="54">
         <v>149.59800000000001</v>
@@ -28130,10 +28130,10 @@
         <v>27821.3</v>
       </c>
       <c r="D56" s="53">
+        <v>27961.1</v>
+      </c>
+      <c r="E56" s="53">
         <v>42443.6</v>
-      </c>
-      <c r="E56" s="53">
-        <v>27961.1</v>
       </c>
       <c r="F56" s="54">
         <v>150.31800000000001</v>
@@ -28183,10 +28183,10 @@
         <v>27944.5</v>
       </c>
       <c r="D57" s="53">
+        <v>28085</v>
+      </c>
+      <c r="E57" s="53">
         <v>42840.800000000003</v>
-      </c>
-      <c r="E57" s="53">
-        <v>28085</v>
       </c>
       <c r="F57" s="54">
         <v>151.042</v>

</xml_diff>